<commit_message>
Updating assertion conditions for both integration and unit mode resources
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
@@ -4275,7 +4275,7 @@
         <v>17</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>16</v>
@@ -4333,7 +4333,7 @@
         <v>17</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>16</v>
@@ -4391,7 +4391,7 @@
         <v>17</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>16</v>
@@ -4449,7 +4449,7 @@
         <v>17</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>16</v>
@@ -6419,7 +6419,7 @@
         <v>17</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>302</v>
@@ -6506,7 +6506,7 @@
         <v>17</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>302</v>
@@ -8369,7 +8369,7 @@
         <v>17</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G196" s="1" t="s">
         <v>356</v>
@@ -8456,7 +8456,7 @@
         <v>17</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>356</v>

</xml_diff>

<commit_message>
Adding integration case to test 662
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3712" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="617">
   <si>
     <t>Class</t>
   </si>
@@ -2212,6 +2212,25 @@
   <si>
     <t>[org.hibernate.SessionFactory : { }
 ]</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.AtomViewImpl</t>
+  </si>
+  <si>
+    <t>buildFeedMetadata
+(Ljava/util/Map;Lcom/rometools/rome/feed/atom/Feed;Ljakarta/servlet/http/HttpServletRequest;)V</t>
+  </si>
+  <si>
+    <t>[java.util.Map&lt;java.lang.String,java.lang.Object&gt; : { "keyFromClassMap" : "0" } 
+, com.rometools.rome.feed.atom.Feed : { "xmlBase" : "string", "categories" : [ { "term" : "string", "scheme" : "string", "schemeResolved" : "string", "label" : "string" } ], "authors" : [ null ], "contributors" : [ null ], "generator" : { "url" : "string", "version" : "string", "value" : "string" }, "icon" : "string", "id" : "string", "logo" : "string", "rights" : "string", "subtitle" : { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" }, "title" : { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" }, "updated" : 1708332767267, "alternateLinks" : [ { "href" : "string", "hrefResolved" : "string", "rel" : "string", "type" : "string", "hreflang" : "string", "title" : "string", "length" : "0" } ], "otherLinks" : [ { "href" : "string", "hrefResolved" : "string", "rel" : "string", "type" : "string", "hreflang" : "string", "title" : "string", "length" : "0" } ], "entries" : [ { "summary" : { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" }, "title" : { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" }, "created" : 1708332767271, "published" : 1708332767271, "updated" : 1708332767271, "source" : null, "alternateLinks" : [ { "href" : "string", "hrefResolved" : "string", "rel" : "string", "type" : "string", "hreflang" : "string", "title" : "string", "length" : "0" } ], "authors" : [ null ], "categories" : [ { "term" : "string", "scheme" : "string", "schemeResolved" : "string", "label" : "string" } ], "contents" : [ { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" } ], "contributors" : [ null ], "foreignMarkup" : [ { "name" : "string", "namespace" : { "prefix" : "string", "uri" : "string" }, "additionalNamespaces" : [ { "prefix" : "string", "uri" : "string" } ], "attributes" : { "attributeData" : [ { "name" : "string", "namespace" : { "prefix" : "string", "uri" : "string" }, "value" : "string", "type" : "UNDECLARED", "specified" : true, "parent" : null } ], "size" : "0", "parent" : null, "modCount" : "0" }, "content" : { "elementData" : [ { "parent" : null, "ctype" : "Comment" } ], "size" : "0", "sizeModCount" : "0", "dataModiCount" : "0", "parent" : null, "modCount" : "0" }, "parent" : null, "ctype" : "Comment" } ], "modules" : [ null ], "otherLinks" : [ { "href" : "string", "hrefResolved" : "string", "rel" : "string", "type" : "string", "hreflang" : "string", "title" : "string", "length" : "0" } ], "id" : "string", "rights" : "string", "xmlBase" : "string" } ], "modules" : [ null ], "info" : { "type" : "string", "value" : "string", "src" : "string", "mode" : "string" }, "language" : "string", "feedType" : "string", "encoding" : "string", "styleSheet" : "string", "foreignMarkup" : [ { "name" : "string", "namespace" : { "prefix" : "string", "uri" : "string" }, "additionalNamespaces" : [ { "prefix" : "string", "uri" : "string" } ], "attributes" : { "attributeData" : [ { "name" : "string", "namespace" : { "prefix" : "string", "uri" : "string" }, "value" : "string", "type" : "UNDECLARED", "specified" : true, "parent" : null } ], "size" : "0", "parent" : null, "modCount" : "0" }, "content" : { "elementData" : [ { "parent" : null, "ctype" : "Comment" } ], "size" : "0", "sizeModCount" : "0", "dataModiCount" : "0", "parent" : null, "modCount" : "0" }, "parent" : null, "ctype" : "Comment" } ] } 
+, jakarta.servlet.http.HttpServletRequest : null 
+]</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"currentRequestAttributes","fileName":"RequestContextHolder.java","lineNumber":131,"nativeMethod":false,"className":"org.springframework.web.context.request.RequestContextHolder"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getUrl","fileName":"SiteUrl.java","lineNumber":14,"nativeMethod":false,"className":"org.unlogged.demo.controller.SiteUrl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"getAbsoluteUrl","fileName":"SiteUrl.java","lineNumber":21,"nativeMethod":false,"className":"org.unlogged.demo.controller.SiteUrl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"setFeedUrl","fileName":"AtomViewImpl.java","lineNumber":49,"nativeMethod":false,"className":"org.unlogged.demo.controller.AtomViewImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"buildFeedMetadata","fileName":"AtomViewImpl.java","lineNumber":33,"nativeMethod":false,"className":"org.unlogged.demo.controller.AtomViewImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":402,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":472,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":69,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.10","methodName":"run","fileName":"Thread.java","lineNumber":840,"nativeMethod":false,"className":"java.lang.Thread"}],"message":"No thread-bound request found: Are you referring to request attributes outside of an actual web request, or processing a request outside of the originally receiving thread? If you are actually operating within a web request and still receive this message, your code is probably running outside of DispatcherServlet: In this case, use RequestContextListener or RequestContextFilter to expose the current request.","suppressed":[],"localizedMessage":"No thread-bound request found: Are you referring to request attributes outside of an actual web request, or processing a request outside of the originally receiving thread? If you are actually operating within a web request and still receive this message, your code is probably running outside of DispatcherServlet: In this case, use RequestContextListener or RequestContextFilter to expose the current request."}</t>
+  </si>
+  <si>
+    <t>#662</t>
   </si>
 </sst>
 </file>
@@ -14988,7 +15007,52 @@
       <c r="W401" s="11"/>
       <c r="X401" s="11"/>
     </row>
-    <row r="402" ht="45.0" customHeight="1"/>
+    <row r="402" ht="45.0" customHeight="1">
+      <c r="A402" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="B402" s="8" t="s">
+        <v>613</v>
+      </c>
+      <c r="C402" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="D402" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E402" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="F402" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G402" s="8" t="s">
+        <v>615</v>
+      </c>
+      <c r="H402" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I402" s="11"/>
+      <c r="J402" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K402" s="11"/>
+      <c r="L402" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="M402" s="11"/>
+      <c r="N402" s="11"/>
+      <c r="O402" s="11"/>
+      <c r="P402" s="11"/>
+      <c r="Q402" s="11"/>
+      <c r="R402" s="11"/>
+      <c r="S402" s="11"/>
+      <c r="T402" s="11"/>
+      <c r="U402" s="11"/>
+      <c r="V402" s="11"/>
+      <c r="W402" s="11"/>
+      <c r="X402" s="11"/>
+    </row>
     <row r="403" ht="45.0" customHeight="1"/>
     <row r="404" ht="45.0" customHeight="1"/>
     <row r="405" ht="45.0" customHeight="1"/>

</xml_diff>

<commit_message>
updating integration test resources for maven demo
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3722" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3731" uniqueCount="621">
   <si>
     <t>Class</t>
   </si>
@@ -2231,6 +2231,19 @@
   </si>
   <si>
     <t>#662</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.jspdemo.wfm.Controllers.UserController</t>
+  </si>
+  <si>
+    <t>getDeepClass
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/DeepClass;</t>
+  </si>
+  <si>
+    <t>Failed to serialize response object of type: org.unlogged.demo.jspdemo.wfm.Models.Entities.DeepClass</t>
+  </si>
+  <si>
+    <t>#684 and #685</t>
   </si>
 </sst>
 </file>
@@ -15053,7 +15066,35 @@
       <c r="W402" s="11"/>
       <c r="X402" s="11"/>
     </row>
-    <row r="403" ht="45.0" customHeight="1"/>
+    <row r="403" ht="45.0" customHeight="1">
+      <c r="A403" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C403" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E403" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F403" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G403" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="J403" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L403" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
     <row r="404" ht="45.0" customHeight="1"/>
     <row r="405" ht="45.0" customHeight="1"/>
     <row r="406" ht="45.0" customHeight="1"/>

</xml_diff>

<commit_message>
adding 82 more replay cases
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3257" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4078" uniqueCount="701">
   <si>
     <t>Class</t>
   </si>
@@ -1945,6 +1945,590 @@
   </si>
   <si>
     <t>#684 and #685</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.VarOpsController</t>
+  </si>
+  <si>
+    <t>primitivesWrapped
+()Ljava/util/List&lt;Ljava/lang/Object;&gt;;</t>
+  </si>
+  <si>
+    <t>[1,1,1.0,1.0,"a","String",["v1","v2","v3"]]</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>getAUser
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;</t>
+  </si>
+  <si>
+    <t>{"user_id":199,"username":"user199","password":"userpass199","email":"user199@gmail.com"}</t>
+  </si>
+  <si>
+    <t>varListAndMap
+()Ljava/util/Map&lt;Ljava/lang/String;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"Even":[{"user_id":14,"username":"UserC","password":"c","email":"userC@gmail.com"},{"user_id":64,"username":"UserE","password":"e","email":"userE@gmail.com"},{"user_id":80,"username":"UserF","password":"f","email":"userF@gmail.com"},{"user_id":24,"username":"UserG","password":"g","email":"userG@gmail.com"}],"Odd":[{"user_id":11,"username":"UserA","password":"a","email":"userA@gmail.com"},{"user_id":23,"username":"UserB","password":"b","email":"userB@gmail.com"},{"user_id":59,"username":"UserD","password":"d","email":"userD@gmail.com"}]}</t>
+  </si>
+  <si>
+    <t>getAsResponseEntity
+()Lorg/springframework/http/ResponseEntity&lt;Ljava/util/Map&lt;Ljava/lang/String;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"Even":[{"user_id":14,"username":"UserC","password":"c","email":"userC@gmail.com"},{"user_id":64,"username":"UserE","password":"e","email":"userE@gmail.com"},{"user_id":80,"username":"UserF","password":"f","email":"userF@gmail.com"},{"user_id":24,"username":"UserG","password":"g","email":"userG@gmail.com"}],"Odd":[{"user_id":11,"username":"UserA","password":"a","email":"userA@gmail.com"},{"user_id":23,"username":"UserB","password":"b","email":"userB@gmail.com"},{"user_id":59,"username":"UserD","password":"d","email":"userD@gmail.com"}]},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>getCustomers
+()Lorg/springframework/http/ResponseEntity&lt;Ljava/util/List&lt;Lorg/unlogged/demo/models/CustomerProfile;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":[{"customerid":1,"customername":"c1","dateofbirth":"dob1","email":"email1","contactnumber":"001","address":"address","referralcodes":["1","2"],"createdDate":"Jun 21, 2024 13:18:02 pm","updatedDate":"Jun 21, 2024 13:18:02 pm"},{"customerid":2,"customername":"c2","dateofbirth":"dob2","email":"email2","contactnumber":"002","address":"address","referralcodes":["1","2"],"createdDate":"Jun 21, 2024 13:18:02 pm","updatedDate":"Jun 21, 2024 13:18:02 pm"}],"status":"OK"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.ValidatorOpsController</t>
+  </si>
+  <si>
+    <t>getValidUser
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;</t>
+  </si>
+  <si>
+    <t>{"user_id":1,"username":"User","password":"password","email":"user@usermail.com"}</t>
+  </si>
+  <si>
+    <t>isDefaultUserVaild
+()Z</t>
+  </si>
+  <si>
+    <t>isUserValid
+(Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;)Z</t>
+  </si>
+  <si>
+    <t>[org.unlogged.demo.jspdemo.wfm.Models.Entities.User : {"user_id":"0","username":"string","password":"string","email":"string"}
+]</t>
+  </si>
+  <si>
+    <t>validateUserV2
+(Lorg/unlogged/demo/models/valid/UserV2;)Ljava/util/Map&lt;Lorg/unlogged/demo/models/valid/UserV2;Ljava/lang/Boolean;&gt;;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.demo.models.valid.UserV2 : {"id":"0","name":"string","email":"string","phoneNumber":"string"}
+]</t>
+  </si>
+  <si>
+    <t>{"UserV2(id=0, name=string, email=string, phoneNumber=string)":true}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.ThreadingOpsController</t>
+  </si>
+  <si>
+    <t>getListofCallables
+()Ljava/util/List&lt;Ljava/util/concurrent/Callable&lt;Ljava/lang/String;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"className": "java.util.ArrayList"}</t>
+  </si>
+  <si>
+    <t>executorServiceCallablesAll
+()Ljava/util/List&lt;Ljava/lang/String;&gt;;</t>
+  </si>
+  <si>
+    <t>["E","E","E"]</t>
+  </si>
+  <si>
+    <t>executorServiceCallablesAny
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>executorServiceRunnable
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>#R1</t>
+  </si>
+  <si>
+    <t>scheduledThread
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>scheduledThreadFixedRate
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>scheduledThreadFixedDelay
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>#R1#R1#R1</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.StreamOpsController</t>
+  </si>
+  <si>
+    <t>getbuilderWithDefaultValues
+()Ljava/util/stream/Stream/Builder&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"className": "java.util.stream.Streams.StreamBuilderImpl"}</t>
+  </si>
+  <si>
+    <t>getUserGroups
+()Ljava/util/List&lt;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[[{"user_id":1,"username":"User1","password":"User1pass","email":"User1@gmail.com"},{"user_id":2,"username":"User2","password":"User2pass","email":"User2@gmail.com"},{"user_id":3,"username":"User3","password":"User3pass","email":"User3@gmail.com"}],[{"user_id":401,"username":"CLP","password":"C401","email":"CLP401@gmail.com"},{"user_id":402,"username":"TRP","password":"T402","email":"TRP402@gmail.com"},{"user_id":403,"username":"DED","password":"D403","email":"DED403@gmail.com"}],[{"user_id":9901,"username":"lck","password":"S???","email":"SL?@gmail.com"},{"user_id":9902,"username":"msc","password":"S117","email":"S117@gmail.com"},{"user_id":9903,"username":"arb","password":"YK04","email":"SHA@gmail.com"}]]</t>
+  </si>
+  <si>
+    <t>getUserList
+()Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>[{"user_id":11,"username":"UserA","password":"a","email":"userA@gmail.com"},{"user_id":23,"username":"UserB","password":"b","email":"userB@gmail.com"},{"user_id":14,"username":"UserC","password":"c","email":"userC@gmail.com"},{"user_id":59,"username":"UserD","password":"d","email":"userD@gmail.com"},{"user_id":64,"username":"UserE","password":"e","email":"userE@gmail.com"},{"user_id":80,"username":"UserF","password":"f","email":"userF@gmail.com"},{"user_id":24,"username":"UserG","password":"g","email":"userG@gmail.com"}]</t>
+  </si>
+  <si>
+    <t>forEachRunParallel
+()Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>[{"user_id":11,"username":"UserA#","password":"a_1459","email":"userA-@gmail.com"},{"user_id":23,"username":"UserB#","password":"b_1459","email":"userB-@gmail.com"},{"user_id":14,"username":"UserC#","password":"C_1397","email":"userC+@gmail.com"},{"user_id":59,"username":"UserD#","password":"d_1459","email":"userD-@gmail.com"},{"user_id":64,"username":"UserE#","password":"E_1397","email":"userE+@gmail.com"},{"user_id":80,"username":"UserF#","password":"F_1397","email":"userF+@gmail.com"},{"user_id":24,"username":"UserG#","password":"G_1397","email":"userG+@gmail.com"}]</t>
+  </si>
+  <si>
+    <t>mapAndCollect
+()Ljava/util/List&lt;Ljava/lang/Long;&gt;;</t>
+  </si>
+  <si>
+    <t>[11,23,14,59,64,80,24]</t>
+  </si>
+  <si>
+    <t>mapSet
+()Ljava/util/Set&lt;Ljava/lang/Long;&gt;;</t>
+  </si>
+  <si>
+    <t>[64,80,23,24,11,59,14]</t>
+  </si>
+  <si>
+    <t>mapVector
+()Ljava/util/Vector&lt;Ljava/lang/Long;&gt;;</t>
+  </si>
+  <si>
+    <t>mapAndFilter
+()Ljava/util/List&lt;Ljava/lang/Long;&gt;;</t>
+  </si>
+  <si>
+    <t>[11,23,59]</t>
+  </si>
+  <si>
+    <t>filterAndFindFirst
+()Ljava/util/Optional&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"user_id":14,"username":"UserC","password":"c","email":"userC@gmail.com"}</t>
+  </si>
+  <si>
+    <t>toArrayCollection_Usernames
+()[Ljava/lang/Object;</t>
+  </si>
+  <si>
+    <t>["UserA","UserB","UserC","UserD","UserE","UserF","UserG"]</t>
+  </si>
+  <si>
+    <t>flatmap_maxId
+()Ljava/util/Optional&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"user_id":9903,"username":"arb","password":"YK04","email":"SHA@gmail.com"}</t>
+  </si>
+  <si>
+    <t>flatmap_minId
+()Ljava/util/Optional&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"user_id":1,"username":"User1","password":"User1pass","email":"User1@gmail.com"}</t>
+  </si>
+  <si>
+    <t>peek_all
+()Ljava/util/List&lt;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>[[{"user_id":1,"username":"User1#","password":"user1pass_1397","email":"user1pass_1397"},{"user_id":2,"username":"User2#","password":"user2pass_1397","email":"user2pass_1397"},{"user_id":3,"username":"User3#","password":"user3pass_1397","email":"user3pass_1397"}],[{"user_id":401,"username":"CLP#","password":"c401_1397","email":"c401_1397"},{"user_id":402,"username":"TRP#","password":"t402_1397","email":"t402_1397"},{"user_id":403,"username":"DED#","password":"d403_1397","email":"d403_1397"}],[{"user_id":9901,"username":"lck#","password":"s???_1397","email":"s???_1397"},{"user_id":9902,"username":"msc#","password":"s117_1397","email":"s117_1397"},{"user_id":9903,"username":"arb#","password":"yk04_1397","email":"yk04_1397"}]]</t>
+  </si>
+  <si>
+    <t>countUsersInGroups
+()J</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>limitUsers
+(I)Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>[int : "5"
+]</t>
+  </si>
+  <si>
+    <t>[{"user_id":1,"username":"User1","password":"User1pass","email":"User1@gmail.com"},{"user_id":2,"username":"User2","password":"User2pass","email":"User2@gmail.com"},{"user_id":3,"username":"User3","password":"User3pass","email":"User3@gmail.com"},{"user_id":401,"username":"CLP","password":"C401","email":"CLP401@gmail.com"},{"user_id":402,"username":"TRP","password":"T402","email":"TRP402@gmail.com"}]</t>
+  </si>
+  <si>
+    <t>distinctUsage
+()Ljava/util/List&lt;Ljava/lang/Integer;&gt;;</t>
+  </si>
+  <si>
+    <t>[2,5,3,4]</t>
+  </si>
+  <si>
+    <t>matchCases
+()Ljava/util/Map&lt;Ljava/lang/String;Ljava/lang/Boolean;&gt;;</t>
+  </si>
+  <si>
+    <t>{"all-false":false,"all-true":true,"any-false":false,"any-true":true,"none-false":false,"none-true":true}</t>
+  </si>
+  <si>
+    <t>reduceUsage
+()Ljava/lang/Long;</t>
+  </si>
+  <si>
+    <t>30918</t>
+  </si>
+  <si>
+    <t>getSortedIdOrder
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>11 &lt; 14 &lt; 23 &lt; 24 &lt; 59 &lt; 64 &lt; 80</t>
+  </si>
+  <si>
+    <t>partitionBy
+()Ljava/util/Map&lt;Ljava/lang/Boolean;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"false":[{"user_id":11,"username":"UserA","password":"a","email":"userA@gmail.com"},{"user_id":23,"username":"UserB","password":"b","email":"userB@gmail.com"},{"user_id":59,"username":"UserD","password":"d","email":"userD@gmail.com"}],"true":[{"user_id":14,"username":"UserC","password":"c","email":"userC@gmail.com"},{"user_id":64,"username":"UserE","password":"e","email":"userE@gmail.com"},{"user_id":80,"username":"UserF","password":"f","email":"userF@gmail.com"},{"user_id":24,"username":"UserG","password":"g","email":"userG@gmail.com"}]}</t>
+  </si>
+  <si>
+    <t>groupBy
+()Ljava/util/Map&lt;Ljava/lang/Character;Ljava/util/List&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;&gt;;</t>
+  </si>
+  <si>
+    <t>{"a":[{"user_id":9903,"username":"arb","password":"YK04","email":"SHA@gmail.com"}],"c":[{"user_id":401,"username":"CLP","password":"C401","email":"CLP401@gmail.com"}],"d":[{"user_id":403,"username":"DED","password":"D403","email":"DED403@gmail.com"}],"t":[{"user_id":402,"username":"TRP","password":"T402","email":"TRP402@gmail.com"}],"u":[{"user_id":1,"username":"User1","password":"User1pass","email":"User1@gmail.com"},{"user_id":2,"username":"User2","password":"User2pass","email":"User2@gmail.com"},{"user_id":3,"username":"User3","password":"User3pass","email":"User3@gmail.com"}],"l":[{"user_id":9901,"username":"lck","password":"S???","email":"SL?@gmail.com"}],"m":[{"user_id":9902,"username":"msc","password":"S117","email":"S117@gmail.com"}]}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.SealedOpsController</t>
+  </si>
+  <si>
+    <t>shapeSerial
+()Lorg/unlogged/demo/models/sealed/Shape;</t>
+  </si>
+  <si>
+    <t>getSquare
+()Lorg/unlogged/demo/models/sealed/Square;</t>
+  </si>
+  <si>
+    <t>{"side":1.0}</t>
+  </si>
+  <si>
+    <t>getRectangle
+()Lorg/unlogged/demo/models/sealed/Rectangle;</t>
+  </si>
+  <si>
+    <t>{"length":1.0,"width":1.0}</t>
+  </si>
+  <si>
+    <t>getFilledRectangle
+()Lorg/unlogged/demo/models/sealed/FilledRectangle;</t>
+  </si>
+  <si>
+    <t>{"length":1.0,"width":1.0,"red":1,"green":1,"blue":1}</t>
+  </si>
+  <si>
+    <t>getRectFromFilled
+()Lorg/unlogged/demo/models/sealed/Rectangle;</t>
+  </si>
+  <si>
+    <t>getCircle
+()Lorg/unlogged/demo/models/sealed/Circle;</t>
+  </si>
+  <si>
+    <t>{"radius":2.0}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.ResponseEntityOps</t>
+  </si>
+  <si>
+    <t>getOkString
+()Lorg/springframework/http/ResponseEntity&lt;Ljava/lang/String;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":"ok","status":"OK"}</t>
+  </si>
+  <si>
+    <t>getOkUser
+()Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"user_id":1,"username":"u1","password":"p1","email":"e1"},"status":"OK"}</t>
+  </si>
+  <si>
+    <t>getUserOf
+()Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"type":"about:blank","title":null,"status":200,"detail":null,"instance":null,"properties":null},"status":200}</t>
+  </si>
+  <si>
+    <t>createWithCode
+()Lorg/springframework/http/ResponseEntity&lt;Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;&gt;;</t>
+  </si>
+  <si>
+    <t>{"headers":{},"body":{"user_id":1,"username":"u1","password":"p1","email":"e1"},"status":"CREATED"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.RecursionController</t>
+  </si>
+  <si>
+    <t>getFactorialOfNumber
+(I)I</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>[int : "10"
+]</t>
+  </si>
+  <si>
+    <t>3628800</t>
+  </si>
+  <si>
+    <t>getFibonacciSeries
+(I)I</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>getIsPalindrome
+(Ljava/lang/String;)Z</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "abba"
+]</t>
+  </si>
+  <si>
+    <t>[java.lang.String : "not"
+]</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.OptionalOpsController</t>
+  </si>
+  <si>
+    <t>getDefaultUser
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;</t>
+  </si>
+  <si>
+    <t>{"user_id":1,"username":"User1","password":"user","email":"user@gmail.com"}</t>
+  </si>
+  <si>
+    <t>getEmptyOptionalUser
+()Lorg/unlogged/demo/models/UserOptional;</t>
+  </si>
+  <si>
+    <t>{"name":null,"email":null,"number":null}</t>
+  </si>
+  <si>
+    <t>getNonEmptyOptionalUser
+()Lorg/unlogged/demo/models/UserOptional;</t>
+  </si>
+  <si>
+    <t>{"name":"a","email":"c","number":"e"}</t>
+  </si>
+  <si>
+    <t>create1
+()Ljava/util/Optional&lt;Ljava/lang/String;&gt;;</t>
+  </si>
+  <si>
+    <t>"default"</t>
+  </si>
+  <si>
+    <t>createNullable
+()Ljava/util/Optional&lt;Ljava/lang/String;&gt;;</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>getPresentStatus
+()Ljava/util/List&lt;Ljava/lang/Boolean;&gt;;</t>
+  </si>
+  <si>
+    <t>[true,false]</t>
+  </si>
+  <si>
+    <t>getEmptyStatus
+()Ljava/util/List&lt;Ljava/lang/Boolean;&gt;;</t>
+  </si>
+  <si>
+    <t>[false,true]</t>
+  </si>
+  <si>
+    <t>ifPresent
+()Ljava/util/concurrent/atomic/AtomicReference&lt;Ljava/lang/String;&gt;;</t>
+  </si>
+  <si>
+    <t>"Ace###"</t>
+  </si>
+  <si>
+    <t>orElseCase
+()Ljava/lang/Object;</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>orElseGet
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;</t>
+  </si>
+  <si>
+    <t>throwOnNull
+()Ljava/lang/Object;</t>
+  </si>
+  <si>
+    <t>{"cause":null,"stackTrace":[{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"orElseThrow","fileName":"Optional.java","lineNumber":403,"nativeMethod":false,"className":"java.util.Optional"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"throwOnNull","fileName":"OptionalOpsController.java","lineNumber":74,"nativeMethod":false,"className":"org.unlogged.demo.controller.OptionalOpsController"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"invoke0","fileName":"NativeMethodAccessorImpl.java","lineNumber":-2,"nativeMethod":true,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"invoke","fileName":"NativeMethodAccessorImpl.java","lineNumber":77,"nativeMethod":false,"className":"jdk.internal.reflect.NativeMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"invoke","fileName":"DelegatingMethodAccessorImpl.java","lineNumber":43,"nativeMethod":false,"className":"jdk.internal.reflect.DelegatingMethodAccessorImpl"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"invoke","fileName":"Method.java","lineNumber":568,"nativeMethod":false,"className":"java.lang.reflect.Method"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommandRaw","fileName":"AgentCommandExecutorImpl.java","lineNumber":407,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"executeCommand","fileName":"AgentCommandExecutorImpl.java","lineNumber":477,"nativeMethod":false,"className":"io.unlogged.AgentCommandExecutorImpl"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"serve","fileName":"AgentCommandServer.java","lineNumber":74,"nativeMethod":false,"className":"io.unlogged.command.AgentCommandServer"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"execute","fileName":"NanoHTTPD.java","lineNumber":945,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$HTTPSession"},{"classLoaderName":"app","moduleName":null,"moduleVersion":null,"methodName":"run","fileName":"NanoHTTPD.java","lineNumber":192,"nativeMethod":false,"className":"fi.iki.elonen.NanoHTTPD$ClientHandler"},{"classLoaderName":null,"moduleName":"java.base","moduleVersion":"17.0.7","methodName":"run","fileName":"Thread.java","lineNumber":833,"nativeMethod":false,"className":"java.lang.Thread"}],"message":null,"suppressed":[],"localizedMessage":null}</t>
+  </si>
+  <si>
+    <t>getUserUsage
+()Lorg/unlogged/demo/jspdemo/wfm/Models/Entities/User;</t>
+  </si>
+  <si>
+    <t>filterUserOptional
+()Ljava/util/List&lt;Ljava/lang/Boolean;&gt;;</t>
+  </si>
+  <si>
+    <t>countNameLength
+()I</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>flatMapUsage
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>chain
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.MongoOpsController</t>
+  </si>
+  <si>
+    <t>insertDefault
+()Lorg/unlogged/demo/models/MongoPojo;</t>
+  </si>
+  <si>
+    <t>{"id":"aaa","name":"Name AAA"}</t>
+  </si>
+  <si>
+    <t>Exception: Write operation error on server localhost:27017. Write error: WriteError{code=11000, message='E11000 duplicate key error collection: test.mongoPojo index: _id_ dup key: { _id: "aaa" }', details={}}.</t>
+  </si>
+  <si>
+    <t>insertNew
+(Lorg/unlogged/demo/models/MongoPojo;)Lorg/unlogged/demo/models/MongoPojo;</t>
+  </si>
+  <si>
+    <t>[org.unlogged.demo.models.MongoPojo : {"id":"string","name":"string"}
+]</t>
+  </si>
+  <si>
+    <t>{"id":"string","name":"string"}</t>
+  </si>
+  <si>
+    <t>getall
+()Ljava/util/List&lt;Lorg/unlogged/demo/models/MongoPojo;&gt;;</t>
+  </si>
+  <si>
+    <t>[{"id":"aaa","name":"Name AAA"},{"id":"string","name":"string"}]</t>
+  </si>
+  <si>
+    <t>getById
+(Ljava/lang/String;)Lorg/unlogged/demo/models/MongoPojo;</t>
+  </si>
+  <si>
+    <t>updatePojo
+(Lorg/unlogged/demo/models/MongoPojo;)Lorg/unlogged/demo/models/MongoPojo;</t>
+  </si>
+  <si>
+    <t>deleteById
+(Ljava/lang/String;)V</t>
+  </si>
+  <si>
+    <t>[{"id":"aaa","name":"Name AAA"}]</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.ModelMapperOpsController</t>
+  </si>
+  <si>
+    <t>getDefaultModel
+()Lorg/unlogged/demo/models/mapper/model/UserModel;</t>
+  </si>
+  <si>
+    <t>{"id":1,"username":"User1","address":{"house":"#144","street":"StreetX","area":"AreaX","city":"CityX","state":"StateX","country":"CountryX","pincode":"PinX"},"contactInformation":{"emails":["user1@gmail.com","user1@yahoo.com"],"numbers":["phone-number-1","phone-number-2"]}}</t>
+  </si>
+  <si>
+    <t>getEmptyUserModelDto
+()Lorg/unlogged/demo/models/mapper/dto/UserModelDto;</t>
+  </si>
+  <si>
+    <t>{"username":null,"phoneNumber":null,"email":null,"address":null}</t>
+  </si>
+  <si>
+    <t>getUserModelMiniDto
+()Lorg/unlogged/demo/models/mapper/dto/UserModelMiniDto;</t>
+  </si>
+  <si>
+    <t>{"id":1,"username":"user1"}</t>
+  </si>
+  <si>
+    <t>getUserModelDto
+()Lorg/unlogged/demo/models/mapper/dto/UserModelDto;</t>
+  </si>
+  <si>
+    <t>{"username":"User1","phoneNumber":null,"email":null,"address":"##144, StateX, AreaX, CityX, StateX, CountryX - Pin-code : PinX"}</t>
+  </si>
+  <si>
+    <t>getUserModelDtoWithProvider
+()Lorg/unlogged/demo/models/mapper/dto/UserModelDto;</t>
+  </si>
+  <si>
+    <t>{"username":null,"phoneNumber":null,"email":null,"address":"##144, StateX, AreaX, CityX, StateX, CountryX - Pin-code : PinX"}</t>
+  </si>
+  <si>
+    <t>getFromConverter
+()Lorg/unlogged/demo/models/mapper/dto/UserModelDto;</t>
+  </si>
+  <si>
+    <t>{"username":"User1","phoneNumber":"phone-number-1","email":"user1@gmail.com","address":"##144, StateX, AreaX, CityX, StateX, CountryX - Pin-code : PinX"}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.controller.GreetingController</t>
+  </si>
+  <si>
+    <t>getGreeting
+()Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>Good Day</t>
   </si>
 </sst>
 </file>
@@ -2002,7 +2586,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2051,6 +2635,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -13278,88 +13865,3534 @@
         <v>534</v>
       </c>
     </row>
-    <row r="356" ht="45.0" customHeight="1"/>
-    <row r="357" ht="45.0" customHeight="1"/>
-    <row r="358" ht="45.0" customHeight="1"/>
-    <row r="359" ht="45.0" customHeight="1"/>
-    <row r="360" ht="45.0" customHeight="1"/>
-    <row r="361" ht="45.0" customHeight="1"/>
-    <row r="362" ht="45.0" customHeight="1"/>
-    <row r="363" ht="45.0" customHeight="1"/>
-    <row r="364" ht="45.0" customHeight="1"/>
-    <row r="365" ht="45.0" customHeight="1"/>
-    <row r="366" ht="45.0" customHeight="1"/>
-    <row r="367" ht="45.0" customHeight="1"/>
-    <row r="368" ht="45.0" customHeight="1"/>
-    <row r="369" ht="45.0" customHeight="1"/>
-    <row r="370" ht="45.0" customHeight="1"/>
-    <row r="371" ht="45.0" customHeight="1"/>
-    <row r="372" ht="45.0" customHeight="1"/>
-    <row r="373" ht="45.0" customHeight="1"/>
-    <row r="374" ht="45.0" customHeight="1"/>
-    <row r="375" ht="45.0" customHeight="1"/>
-    <row r="376" ht="45.0" customHeight="1"/>
-    <row r="377" ht="45.0" customHeight="1"/>
-    <row r="378" ht="45.0" customHeight="1"/>
-    <row r="379" ht="45.0" customHeight="1"/>
-    <row r="380" ht="45.0" customHeight="1"/>
-    <row r="381" ht="45.0" customHeight="1"/>
-    <row r="382" ht="45.0" customHeight="1"/>
-    <row r="383" ht="45.0" customHeight="1"/>
-    <row r="384" ht="45.0" customHeight="1"/>
-    <row r="385" ht="45.0" customHeight="1"/>
-    <row r="386" ht="45.0" customHeight="1"/>
-    <row r="387" ht="45.0" customHeight="1"/>
-    <row r="388" ht="45.0" customHeight="1"/>
-    <row r="389" ht="45.0" customHeight="1"/>
-    <row r="390" ht="45.0" customHeight="1"/>
-    <row r="391" ht="45.0" customHeight="1"/>
-    <row r="392" ht="45.0" customHeight="1"/>
-    <row r="393" ht="45.0" customHeight="1"/>
-    <row r="394" ht="45.0" customHeight="1"/>
-    <row r="395" ht="45.0" customHeight="1"/>
-    <row r="396" ht="45.0" customHeight="1"/>
-    <row r="397" ht="45.0" customHeight="1"/>
-    <row r="398" ht="45.0" customHeight="1"/>
-    <row r="399" ht="45.0" customHeight="1"/>
-    <row r="400" ht="45.0" customHeight="1"/>
-    <row r="401" ht="45.0" customHeight="1"/>
-    <row r="402" ht="45.0" customHeight="1"/>
-    <row r="403" ht="45.0" customHeight="1"/>
-    <row r="404" ht="45.0" customHeight="1"/>
-    <row r="405" ht="45.0" customHeight="1"/>
-    <row r="406" ht="45.0" customHeight="1"/>
-    <row r="407" ht="45.0" customHeight="1"/>
-    <row r="408" ht="45.0" customHeight="1"/>
-    <row r="409" ht="45.0" customHeight="1"/>
-    <row r="410" ht="45.0" customHeight="1"/>
-    <row r="411" ht="45.0" customHeight="1"/>
-    <row r="412" ht="45.0" customHeight="1"/>
-    <row r="413" ht="45.0" customHeight="1"/>
-    <row r="414" ht="45.0" customHeight="1"/>
-    <row r="415" ht="45.0" customHeight="1"/>
-    <row r="416" ht="45.0" customHeight="1"/>
-    <row r="417" ht="45.0" customHeight="1"/>
-    <row r="418" ht="45.0" customHeight="1"/>
-    <row r="419" ht="45.0" customHeight="1"/>
-    <row r="420" ht="45.0" customHeight="1"/>
-    <row r="421" ht="45.0" customHeight="1"/>
-    <row r="422" ht="45.0" customHeight="1"/>
-    <row r="423" ht="45.0" customHeight="1"/>
-    <row r="424" ht="45.0" customHeight="1"/>
-    <row r="425" ht="45.0" customHeight="1"/>
-    <row r="426" ht="45.0" customHeight="1"/>
-    <row r="427" ht="45.0" customHeight="1"/>
-    <row r="428" ht="45.0" customHeight="1"/>
-    <row r="429" ht="45.0" customHeight="1"/>
-    <row r="430" ht="45.0" customHeight="1"/>
-    <row r="431" ht="45.0" customHeight="1"/>
-    <row r="432" ht="45.0" customHeight="1"/>
-    <row r="433" ht="45.0" customHeight="1"/>
-    <row r="434" ht="45.0" customHeight="1"/>
-    <row r="435" ht="45.0" customHeight="1"/>
-    <row r="436" ht="45.0" customHeight="1"/>
-    <row r="437" ht="45.0" customHeight="1"/>
+    <row r="356" ht="45.0" customHeight="1">
+      <c r="A356" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B356" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D356" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E356" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F356" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G356" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="H356" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I356" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J356" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K356" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L356" s="3"/>
+      <c r="M356" s="3"/>
+      <c r="N356" s="3"/>
+      <c r="O356" s="3"/>
+      <c r="P356" s="3"/>
+      <c r="Q356" s="3"/>
+      <c r="R356" s="3"/>
+      <c r="S356" s="3"/>
+      <c r="T356" s="3"/>
+      <c r="U356" s="3"/>
+    </row>
+    <row r="357" ht="45.0" customHeight="1">
+      <c r="A357" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B357" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D357" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E357" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F357" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G357" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="H357" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I357" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J357" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K357" s="3"/>
+      <c r="L357" s="3"/>
+      <c r="M357" s="3"/>
+      <c r="N357" s="3"/>
+      <c r="O357" s="3"/>
+      <c r="P357" s="3"/>
+      <c r="Q357" s="3"/>
+      <c r="R357" s="3"/>
+      <c r="S357" s="3"/>
+      <c r="T357" s="3"/>
+      <c r="U357" s="3"/>
+    </row>
+    <row r="358" ht="45.0" customHeight="1">
+      <c r="A358" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B358" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="C358" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D358" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E358" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F358" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G358" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="H358" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I358" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J358" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K358" s="3"/>
+      <c r="L358" s="3"/>
+      <c r="M358" s="3"/>
+      <c r="N358" s="3"/>
+      <c r="O358" s="3"/>
+      <c r="P358" s="3"/>
+      <c r="Q358" s="3"/>
+      <c r="R358" s="3"/>
+      <c r="S358" s="3"/>
+      <c r="T358" s="3"/>
+      <c r="U358" s="3"/>
+    </row>
+    <row r="359" ht="45.0" customHeight="1">
+      <c r="A359" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B359" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C359" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D359" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E359" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F359" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G359" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="H359" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I359" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J359" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K359" s="3"/>
+      <c r="L359" s="3"/>
+      <c r="M359" s="3"/>
+      <c r="N359" s="3"/>
+      <c r="O359" s="3"/>
+      <c r="P359" s="3"/>
+      <c r="Q359" s="3"/>
+      <c r="R359" s="3"/>
+      <c r="S359" s="3"/>
+      <c r="T359" s="3"/>
+      <c r="U359" s="3"/>
+    </row>
+    <row r="360" ht="45.0" customHeight="1">
+      <c r="A360" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="C360" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D360" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E360" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F360" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G360" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="H360" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I360" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J360" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K360" s="3"/>
+      <c r="L360" s="3"/>
+      <c r="M360" s="3"/>
+      <c r="N360" s="3"/>
+      <c r="O360" s="3"/>
+      <c r="P360" s="3"/>
+      <c r="Q360" s="3"/>
+      <c r="R360" s="3"/>
+      <c r="S360" s="3"/>
+      <c r="T360" s="3"/>
+      <c r="U360" s="3"/>
+    </row>
+    <row r="361" ht="45.0" customHeight="1">
+      <c r="A361" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D361" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E361" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F361" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G361" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="H361" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I361" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J361" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K361" s="3"/>
+      <c r="L361" s="3"/>
+      <c r="M361" s="3"/>
+      <c r="N361" s="3"/>
+      <c r="O361" s="3"/>
+      <c r="P361" s="3"/>
+      <c r="Q361" s="3"/>
+      <c r="R361" s="3"/>
+      <c r="S361" s="3"/>
+      <c r="T361" s="3"/>
+      <c r="U361" s="3"/>
+    </row>
+    <row r="362" ht="45.0" customHeight="1">
+      <c r="A362" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B362" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D362" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E362" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F362" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G362" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H362" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I362" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J362" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K362" s="3"/>
+      <c r="L362" s="3"/>
+      <c r="M362" s="3"/>
+      <c r="N362" s="3"/>
+      <c r="O362" s="3"/>
+      <c r="P362" s="3"/>
+      <c r="Q362" s="3"/>
+      <c r="R362" s="3"/>
+      <c r="S362" s="3"/>
+      <c r="T362" s="3"/>
+      <c r="U362" s="3"/>
+    </row>
+    <row r="363" ht="45.0" customHeight="1">
+      <c r="A363" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B363" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D363" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E363" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="F363" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G363" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H363" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I363" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J363" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K363" s="3"/>
+      <c r="L363" s="3"/>
+      <c r="M363" s="3"/>
+      <c r="N363" s="3"/>
+      <c r="O363" s="3"/>
+      <c r="P363" s="3"/>
+      <c r="Q363" s="3"/>
+      <c r="R363" s="3"/>
+      <c r="S363" s="3"/>
+      <c r="T363" s="3"/>
+      <c r="U363" s="3"/>
+    </row>
+    <row r="364" ht="45.0" customHeight="1">
+      <c r="A364" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D364" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E364" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G364" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="H364" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I364" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J364" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K364" s="3"/>
+      <c r="L364" s="3"/>
+      <c r="M364" s="3"/>
+      <c r="N364" s="3"/>
+      <c r="O364" s="3"/>
+      <c r="P364" s="3"/>
+      <c r="Q364" s="3"/>
+      <c r="R364" s="3"/>
+      <c r="S364" s="3"/>
+      <c r="T364" s="3"/>
+      <c r="U364" s="3"/>
+    </row>
+    <row r="365" ht="45.0" customHeight="1">
+      <c r="A365" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B365" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D365" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E365" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F365" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G365" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="H365" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I365" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J365" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K365" s="3"/>
+      <c r="L365" s="3"/>
+      <c r="M365" s="3"/>
+      <c r="N365" s="3"/>
+      <c r="O365" s="3"/>
+      <c r="P365" s="3"/>
+      <c r="Q365" s="3"/>
+      <c r="R365" s="3"/>
+      <c r="S365" s="3"/>
+      <c r="T365" s="3"/>
+      <c r="U365" s="3"/>
+    </row>
+    <row r="366" ht="45.0" customHeight="1">
+      <c r="A366" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B366" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D366" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E366" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F366" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G366" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="H366" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I366" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J366" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K366" s="3"/>
+      <c r="L366" s="3"/>
+      <c r="M366" s="3"/>
+      <c r="N366" s="3"/>
+      <c r="O366" s="3"/>
+      <c r="P366" s="3"/>
+      <c r="Q366" s="3"/>
+      <c r="R366" s="3"/>
+      <c r="S366" s="3"/>
+      <c r="T366" s="3"/>
+      <c r="U366" s="3"/>
+    </row>
+    <row r="367" ht="45.0" customHeight="1">
+      <c r="A367" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B367" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="C367" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D367" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E367" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F367" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G367" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="H367" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I367" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J367" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K367" s="3"/>
+      <c r="L367" s="3"/>
+      <c r="M367" s="3"/>
+      <c r="N367" s="3"/>
+      <c r="O367" s="3"/>
+      <c r="P367" s="3"/>
+      <c r="Q367" s="3"/>
+      <c r="R367" s="3"/>
+      <c r="S367" s="3"/>
+      <c r="T367" s="3"/>
+      <c r="U367" s="3"/>
+    </row>
+    <row r="368" ht="45.0" customHeight="1">
+      <c r="A368" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C368" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D368" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E368" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F368" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G368" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="H368" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I368" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J368" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K368" s="3"/>
+      <c r="L368" s="3"/>
+      <c r="M368" s="3"/>
+      <c r="N368" s="3"/>
+      <c r="O368" s="3"/>
+      <c r="P368" s="3"/>
+      <c r="Q368" s="3"/>
+      <c r="R368" s="3"/>
+      <c r="S368" s="3"/>
+      <c r="T368" s="3"/>
+      <c r="U368" s="3"/>
+    </row>
+    <row r="369" ht="45.0" customHeight="1">
+      <c r="A369" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B369" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="C369" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D369" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E369" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F369" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G369" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="H369" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I369" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J369" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K369" s="3"/>
+      <c r="L369" s="3"/>
+      <c r="M369" s="3"/>
+      <c r="N369" s="3"/>
+      <c r="O369" s="3"/>
+      <c r="P369" s="3"/>
+      <c r="Q369" s="3"/>
+      <c r="R369" s="3"/>
+      <c r="S369" s="3"/>
+      <c r="T369" s="3"/>
+      <c r="U369" s="3"/>
+    </row>
+    <row r="370" ht="45.0" customHeight="1">
+      <c r="A370" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="C370" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D370" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E370" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F370" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G370" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="H370" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I370" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J370" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K370" s="3"/>
+      <c r="L370" s="3"/>
+      <c r="M370" s="3"/>
+      <c r="N370" s="3"/>
+      <c r="O370" s="3"/>
+      <c r="P370" s="3"/>
+      <c r="Q370" s="3"/>
+      <c r="R370" s="3"/>
+      <c r="S370" s="3"/>
+      <c r="T370" s="3"/>
+      <c r="U370" s="3"/>
+    </row>
+    <row r="371" ht="45.0" customHeight="1">
+      <c r="A371" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="B371" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="C371" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D371" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E371" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F371" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G371" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="H371" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I371" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J371" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K371" s="3"/>
+      <c r="L371" s="3"/>
+      <c r="M371" s="3"/>
+      <c r="N371" s="3"/>
+      <c r="O371" s="3"/>
+      <c r="P371" s="3"/>
+      <c r="Q371" s="3"/>
+      <c r="R371" s="3"/>
+      <c r="S371" s="3"/>
+      <c r="T371" s="3"/>
+      <c r="U371" s="3"/>
+    </row>
+    <row r="372" ht="45.0" customHeight="1">
+      <c r="A372" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B372" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="C372" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D372" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E372" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F372" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G372" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="H372" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I372" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J372" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K372" s="3"/>
+      <c r="L372" s="3"/>
+      <c r="M372" s="3"/>
+      <c r="N372" s="3"/>
+      <c r="O372" s="3"/>
+      <c r="P372" s="3"/>
+      <c r="Q372" s="3"/>
+      <c r="R372" s="3"/>
+      <c r="S372" s="3"/>
+      <c r="T372" s="3"/>
+      <c r="U372" s="3"/>
+    </row>
+    <row r="373" ht="45.0" customHeight="1">
+      <c r="A373" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B373" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="C373" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D373" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E373" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F373" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G373" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="H373" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I373" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J373" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K373" s="3"/>
+      <c r="L373" s="3"/>
+      <c r="M373" s="3"/>
+      <c r="N373" s="3"/>
+      <c r="O373" s="3"/>
+      <c r="P373" s="3"/>
+      <c r="Q373" s="3"/>
+      <c r="R373" s="3"/>
+      <c r="S373" s="3"/>
+      <c r="T373" s="3"/>
+      <c r="U373" s="3"/>
+    </row>
+    <row r="374" ht="45.0" customHeight="1">
+      <c r="A374" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B374" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="C374" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D374" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E374" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F374" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G374" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="H374" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I374" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J374" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K374" s="3"/>
+      <c r="L374" s="3"/>
+      <c r="M374" s="3"/>
+      <c r="N374" s="3"/>
+      <c r="O374" s="3"/>
+      <c r="P374" s="3"/>
+      <c r="Q374" s="3"/>
+      <c r="R374" s="3"/>
+      <c r="S374" s="3"/>
+      <c r="T374" s="3"/>
+      <c r="U374" s="3"/>
+    </row>
+    <row r="375" ht="45.0" customHeight="1">
+      <c r="A375" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B375" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C375" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D375" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E375" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F375" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G375" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="H375" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I375" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J375" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K375" s="3"/>
+      <c r="L375" s="3"/>
+      <c r="M375" s="3"/>
+      <c r="N375" s="3"/>
+      <c r="O375" s="3"/>
+      <c r="P375" s="3"/>
+      <c r="Q375" s="3"/>
+      <c r="R375" s="3"/>
+      <c r="S375" s="3"/>
+      <c r="T375" s="3"/>
+      <c r="U375" s="3"/>
+    </row>
+    <row r="376" ht="45.0" customHeight="1">
+      <c r="A376" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B376" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="C376" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D376" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E376" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F376" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G376" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H376" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I376" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J376" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K376" s="3"/>
+      <c r="L376" s="3"/>
+      <c r="M376" s="3"/>
+      <c r="N376" s="3"/>
+      <c r="O376" s="3"/>
+      <c r="P376" s="3"/>
+      <c r="Q376" s="3"/>
+      <c r="R376" s="3"/>
+      <c r="S376" s="3"/>
+      <c r="T376" s="3"/>
+      <c r="U376" s="3"/>
+    </row>
+    <row r="377" ht="45.0" customHeight="1">
+      <c r="A377" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B377" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="C377" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D377" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E377" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F377" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G377" s="3" t="s">
+        <v>581</v>
+      </c>
+      <c r="H377" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I377" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J377" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K377" s="3"/>
+      <c r="L377" s="3"/>
+      <c r="M377" s="3"/>
+      <c r="N377" s="3"/>
+      <c r="O377" s="3"/>
+      <c r="P377" s="3"/>
+      <c r="Q377" s="3"/>
+      <c r="R377" s="3"/>
+      <c r="S377" s="3"/>
+      <c r="T377" s="3"/>
+      <c r="U377" s="3"/>
+    </row>
+    <row r="378" ht="45.0" customHeight="1">
+      <c r="A378" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B378" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C378" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D378" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E378" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F378" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G378" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="H378" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I378" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J378" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K378" s="3"/>
+      <c r="L378" s="3"/>
+      <c r="M378" s="3"/>
+      <c r="N378" s="3"/>
+      <c r="O378" s="3"/>
+      <c r="P378" s="3"/>
+      <c r="Q378" s="3"/>
+      <c r="R378" s="3"/>
+      <c r="S378" s="3"/>
+      <c r="T378" s="3"/>
+      <c r="U378" s="3"/>
+    </row>
+    <row r="379" ht="45.0" customHeight="1">
+      <c r="A379" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B379" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="C379" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D379" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E379" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F379" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G379" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="H379" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I379" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J379" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K379" s="3"/>
+      <c r="L379" s="3"/>
+      <c r="M379" s="3"/>
+      <c r="N379" s="3"/>
+      <c r="O379" s="3"/>
+      <c r="P379" s="3"/>
+      <c r="Q379" s="3"/>
+      <c r="R379" s="3"/>
+      <c r="S379" s="3"/>
+      <c r="T379" s="3"/>
+      <c r="U379" s="3"/>
+    </row>
+    <row r="380" ht="45.0" customHeight="1">
+      <c r="A380" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B380" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C380" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D380" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E380" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F380" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G380" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="H380" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I380" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J380" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K380" s="3"/>
+      <c r="L380" s="3"/>
+      <c r="M380" s="3"/>
+      <c r="N380" s="3"/>
+      <c r="O380" s="3"/>
+      <c r="P380" s="3"/>
+      <c r="Q380" s="3"/>
+      <c r="R380" s="3"/>
+      <c r="S380" s="3"/>
+      <c r="T380" s="3"/>
+      <c r="U380" s="3"/>
+    </row>
+    <row r="381" ht="45.0" customHeight="1">
+      <c r="A381" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="C381" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D381" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E381" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F381" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G381" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="H381" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I381" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J381" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K381" s="3"/>
+      <c r="L381" s="3"/>
+      <c r="M381" s="3"/>
+      <c r="N381" s="3"/>
+      <c r="O381" s="3"/>
+      <c r="P381" s="3"/>
+      <c r="Q381" s="3"/>
+      <c r="R381" s="3"/>
+      <c r="S381" s="3"/>
+      <c r="T381" s="3"/>
+      <c r="U381" s="3"/>
+    </row>
+    <row r="382" ht="45.0" customHeight="1">
+      <c r="A382" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="C382" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D382" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E382" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F382" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G382" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="H382" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I382" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J382" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K382" s="3"/>
+      <c r="L382" s="3"/>
+      <c r="M382" s="3"/>
+      <c r="N382" s="3"/>
+      <c r="O382" s="3"/>
+      <c r="P382" s="3"/>
+      <c r="Q382" s="3"/>
+      <c r="R382" s="3"/>
+      <c r="S382" s="3"/>
+      <c r="T382" s="3"/>
+      <c r="U382" s="3"/>
+    </row>
+    <row r="383" ht="45.0" customHeight="1">
+      <c r="A383" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B383" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="C383" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D383" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E383" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F383" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G383" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="H383" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I383" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J383" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K383" s="3"/>
+      <c r="L383" s="3"/>
+      <c r="M383" s="3"/>
+      <c r="N383" s="3"/>
+      <c r="O383" s="3"/>
+      <c r="P383" s="3"/>
+      <c r="Q383" s="3"/>
+      <c r="R383" s="3"/>
+      <c r="S383" s="3"/>
+      <c r="T383" s="3"/>
+      <c r="U383" s="3"/>
+    </row>
+    <row r="384" ht="45.0" customHeight="1">
+      <c r="A384" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C384" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D384" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E384" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F384" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G384" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="H384" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I384" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J384" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K384" s="3"/>
+      <c r="L384" s="3"/>
+      <c r="M384" s="3"/>
+      <c r="N384" s="3"/>
+      <c r="O384" s="3"/>
+      <c r="P384" s="3"/>
+      <c r="Q384" s="3"/>
+      <c r="R384" s="3"/>
+      <c r="S384" s="3"/>
+      <c r="T384" s="3"/>
+      <c r="U384" s="3"/>
+    </row>
+    <row r="385" ht="45.0" customHeight="1">
+      <c r="A385" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B385" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="C385" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D385" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E385" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F385" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G385" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="H385" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I385" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J385" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K385" s="3"/>
+      <c r="L385" s="3"/>
+      <c r="M385" s="3"/>
+      <c r="N385" s="3"/>
+      <c r="O385" s="3"/>
+      <c r="P385" s="3"/>
+      <c r="Q385" s="3"/>
+      <c r="R385" s="3"/>
+      <c r="S385" s="3"/>
+      <c r="T385" s="3"/>
+      <c r="U385" s="3"/>
+    </row>
+    <row r="386" ht="45.0" customHeight="1">
+      <c r="A386" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B386" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="C386" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D386" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E386" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="F386" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G386" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="H386" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I386" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J386" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K386" s="3"/>
+      <c r="L386" s="3"/>
+      <c r="M386" s="3"/>
+      <c r="N386" s="3"/>
+      <c r="O386" s="3"/>
+      <c r="P386" s="3"/>
+      <c r="Q386" s="3"/>
+      <c r="R386" s="3"/>
+      <c r="S386" s="3"/>
+      <c r="T386" s="3"/>
+      <c r="U386" s="3"/>
+    </row>
+    <row r="387" ht="45.0" customHeight="1">
+      <c r="A387" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B387" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C387" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D387" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E387" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F387" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G387" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="H387" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I387" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J387" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K387" s="3"/>
+      <c r="L387" s="3"/>
+      <c r="M387" s="3"/>
+      <c r="N387" s="3"/>
+      <c r="O387" s="3"/>
+      <c r="P387" s="3"/>
+      <c r="Q387" s="3"/>
+      <c r="R387" s="3"/>
+      <c r="S387" s="3"/>
+      <c r="T387" s="3"/>
+      <c r="U387" s="3"/>
+    </row>
+    <row r="388" ht="45.0" customHeight="1">
+      <c r="A388" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B388" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C388" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D388" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E388" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F388" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G388" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H388" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I388" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J388" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K388" s="3"/>
+      <c r="L388" s="3"/>
+      <c r="M388" s="3"/>
+      <c r="N388" s="3"/>
+      <c r="O388" s="3"/>
+      <c r="P388" s="3"/>
+      <c r="Q388" s="3"/>
+      <c r="R388" s="3"/>
+      <c r="S388" s="3"/>
+      <c r="T388" s="3"/>
+      <c r="U388" s="3"/>
+    </row>
+    <row r="389" ht="45.0" customHeight="1">
+      <c r="A389" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B389" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="C389" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D389" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E389" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F389" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G389" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="H389" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I389" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J389" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K389" s="3"/>
+      <c r="L389" s="3"/>
+      <c r="M389" s="3"/>
+      <c r="N389" s="3"/>
+      <c r="O389" s="3"/>
+      <c r="P389" s="3"/>
+      <c r="Q389" s="3"/>
+      <c r="R389" s="3"/>
+      <c r="S389" s="3"/>
+      <c r="T389" s="3"/>
+      <c r="U389" s="3"/>
+    </row>
+    <row r="390" ht="45.0" customHeight="1">
+      <c r="A390" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B390" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="C390" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D390" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E390" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F390" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G390" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="H390" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I390" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J390" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K390" s="3"/>
+      <c r="L390" s="3"/>
+      <c r="M390" s="3"/>
+      <c r="N390" s="3"/>
+      <c r="O390" s="3"/>
+      <c r="P390" s="3"/>
+      <c r="Q390" s="3"/>
+      <c r="R390" s="3"/>
+      <c r="S390" s="3"/>
+      <c r="T390" s="3"/>
+      <c r="U390" s="3"/>
+    </row>
+    <row r="391" ht="45.0" customHeight="1">
+      <c r="A391" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B391" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="C391" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D391" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E391" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F391" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G391" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="H391" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I391" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J391" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K391" s="3"/>
+      <c r="L391" s="3"/>
+      <c r="M391" s="3"/>
+      <c r="N391" s="3"/>
+      <c r="O391" s="3"/>
+      <c r="P391" s="3"/>
+      <c r="Q391" s="3"/>
+      <c r="R391" s="3"/>
+      <c r="S391" s="3"/>
+      <c r="T391" s="3"/>
+      <c r="U391" s="3"/>
+    </row>
+    <row r="392" ht="45.0" customHeight="1">
+      <c r="A392" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="B392" s="3" t="s">
+        <v>610</v>
+      </c>
+      <c r="C392" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D392" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E392" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F392" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G392" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="H392" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I392" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J392" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K392" s="3"/>
+      <c r="L392" s="3"/>
+      <c r="M392" s="3"/>
+      <c r="N392" s="3"/>
+      <c r="O392" s="3"/>
+      <c r="P392" s="3"/>
+      <c r="Q392" s="3"/>
+      <c r="R392" s="3"/>
+      <c r="S392" s="3"/>
+      <c r="T392" s="3"/>
+      <c r="U392" s="3"/>
+    </row>
+    <row r="393" ht="45.0" customHeight="1">
+      <c r="A393" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B393" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="C393" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D393" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E393" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F393" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G393" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="H393" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I393" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J393" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K393" s="3"/>
+      <c r="L393" s="3"/>
+      <c r="M393" s="3"/>
+      <c r="N393" s="3"/>
+      <c r="O393" s="3"/>
+      <c r="P393" s="3"/>
+      <c r="Q393" s="3"/>
+      <c r="R393" s="3"/>
+      <c r="S393" s="3"/>
+      <c r="T393" s="3"/>
+      <c r="U393" s="3"/>
+    </row>
+    <row r="394" ht="45.0" customHeight="1">
+      <c r="A394" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B394" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="C394" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D394" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E394" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F394" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G394" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="H394" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I394" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J394" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K394" s="3"/>
+      <c r="L394" s="3"/>
+      <c r="M394" s="3"/>
+      <c r="N394" s="3"/>
+      <c r="O394" s="3"/>
+      <c r="P394" s="3"/>
+      <c r="Q394" s="3"/>
+      <c r="R394" s="3"/>
+      <c r="S394" s="3"/>
+      <c r="T394" s="3"/>
+      <c r="U394" s="3"/>
+    </row>
+    <row r="395" ht="45.0" customHeight="1">
+      <c r="A395" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B395" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="C395" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D395" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E395" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F395" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G395" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="H395" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I395" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J395" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K395" s="3"/>
+      <c r="L395" s="3"/>
+      <c r="M395" s="3"/>
+      <c r="N395" s="3"/>
+      <c r="O395" s="3"/>
+      <c r="P395" s="3"/>
+      <c r="Q395" s="3"/>
+      <c r="R395" s="3"/>
+      <c r="S395" s="3"/>
+      <c r="T395" s="3"/>
+      <c r="U395" s="3"/>
+    </row>
+    <row r="396" ht="45.0" customHeight="1">
+      <c r="A396" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B396" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="C396" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D396" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E396" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F396" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G396" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="H396" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I396" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J396" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K396" s="3"/>
+      <c r="L396" s="3"/>
+      <c r="M396" s="3"/>
+      <c r="N396" s="3"/>
+      <c r="O396" s="3"/>
+      <c r="P396" s="3"/>
+      <c r="Q396" s="3"/>
+      <c r="R396" s="3"/>
+      <c r="S396" s="3"/>
+      <c r="T396" s="3"/>
+      <c r="U396" s="3"/>
+    </row>
+    <row r="397" ht="45.0" customHeight="1">
+      <c r="A397" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B397" s="3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C397" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D397" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E397" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F397" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G397" s="3" t="s">
+        <v>619</v>
+      </c>
+      <c r="H397" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I397" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J397" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K397" s="3"/>
+      <c r="L397" s="3"/>
+      <c r="M397" s="3"/>
+      <c r="N397" s="3"/>
+      <c r="O397" s="3"/>
+      <c r="P397" s="3"/>
+      <c r="Q397" s="3"/>
+      <c r="R397" s="3"/>
+      <c r="S397" s="3"/>
+      <c r="T397" s="3"/>
+      <c r="U397" s="3"/>
+    </row>
+    <row r="398" ht="45.0" customHeight="1">
+      <c r="A398" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="B398" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C398" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="D398" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E398" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F398" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G398" s="3" t="s">
+        <v>622</v>
+      </c>
+      <c r="H398" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I398" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J398" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K398" s="3"/>
+      <c r="L398" s="3"/>
+      <c r="M398" s="3"/>
+      <c r="N398" s="3"/>
+      <c r="O398" s="3"/>
+      <c r="P398" s="3"/>
+      <c r="Q398" s="3"/>
+      <c r="R398" s="3"/>
+      <c r="S398" s="3"/>
+      <c r="T398" s="3"/>
+      <c r="U398" s="3"/>
+    </row>
+    <row r="399" ht="45.0" customHeight="1">
+      <c r="A399" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B399" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="C399" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D399" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E399" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F399" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G399" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="H399" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I399" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J399" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K399" s="3"/>
+      <c r="L399" s="3"/>
+      <c r="M399" s="3"/>
+      <c r="N399" s="3"/>
+      <c r="O399" s="3"/>
+      <c r="P399" s="3"/>
+      <c r="Q399" s="3"/>
+      <c r="R399" s="3"/>
+      <c r="S399" s="3"/>
+      <c r="T399" s="3"/>
+      <c r="U399" s="3"/>
+    </row>
+    <row r="400" ht="45.0" customHeight="1">
+      <c r="A400" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B400" s="3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C400" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D400" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E400" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F400" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G400" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="H400" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I400" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J400" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K400" s="3"/>
+      <c r="L400" s="3"/>
+      <c r="M400" s="3"/>
+      <c r="N400" s="3"/>
+      <c r="O400" s="3"/>
+      <c r="P400" s="3"/>
+      <c r="Q400" s="3"/>
+      <c r="R400" s="3"/>
+      <c r="S400" s="3"/>
+      <c r="T400" s="3"/>
+      <c r="U400" s="3"/>
+    </row>
+    <row r="401" ht="45.0" customHeight="1">
+      <c r="A401" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B401" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="C401" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D401" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E401" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F401" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G401" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="H401" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I401" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J401" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K401" s="3"/>
+      <c r="L401" s="3"/>
+      <c r="M401" s="3"/>
+      <c r="N401" s="3"/>
+      <c r="O401" s="3"/>
+      <c r="P401" s="3"/>
+      <c r="Q401" s="3"/>
+      <c r="R401" s="3"/>
+      <c r="S401" s="3"/>
+      <c r="T401" s="3"/>
+      <c r="U401" s="3"/>
+    </row>
+    <row r="402" ht="45.0" customHeight="1">
+      <c r="A402" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="B402" s="3" t="s">
+        <v>630</v>
+      </c>
+      <c r="C402" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D402" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E402" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F402" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G402" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="H402" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I402" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J402" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K402" s="3"/>
+      <c r="L402" s="3"/>
+      <c r="M402" s="3"/>
+      <c r="N402" s="3"/>
+      <c r="O402" s="3"/>
+      <c r="P402" s="3"/>
+      <c r="Q402" s="3"/>
+      <c r="R402" s="3"/>
+      <c r="S402" s="3"/>
+      <c r="T402" s="3"/>
+      <c r="U402" s="3"/>
+    </row>
+    <row r="403" ht="45.0" customHeight="1">
+      <c r="A403" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B403" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C403" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="D403" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E403" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="F403" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G403" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="H403" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I403" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J403" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K403" s="3"/>
+      <c r="L403" s="3"/>
+      <c r="M403" s="3"/>
+      <c r="N403" s="3"/>
+      <c r="O403" s="3"/>
+      <c r="P403" s="3"/>
+      <c r="Q403" s="3"/>
+      <c r="R403" s="3"/>
+      <c r="S403" s="3"/>
+      <c r="T403" s="3"/>
+      <c r="U403" s="3"/>
+    </row>
+    <row r="404" ht="45.0" customHeight="1">
+      <c r="A404" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B404" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="C404" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="D404" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E404" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="F404" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G404" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="H404" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I404" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J404" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K404" s="3"/>
+      <c r="L404" s="3"/>
+      <c r="M404" s="3"/>
+      <c r="N404" s="3"/>
+      <c r="O404" s="3"/>
+      <c r="P404" s="3"/>
+      <c r="Q404" s="3"/>
+      <c r="R404" s="3"/>
+      <c r="S404" s="3"/>
+      <c r="T404" s="3"/>
+      <c r="U404" s="3"/>
+    </row>
+    <row r="405" ht="45.0" customHeight="1">
+      <c r="A405" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B405" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="C405" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="D405" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E405" s="3" t="s">
+        <v>635</v>
+      </c>
+      <c r="F405" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G405" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="H405" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I405" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J405" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K405" s="3"/>
+      <c r="L405" s="3"/>
+      <c r="M405" s="3"/>
+      <c r="N405" s="3"/>
+      <c r="O405" s="3"/>
+      <c r="P405" s="3"/>
+      <c r="Q405" s="3"/>
+      <c r="R405" s="3"/>
+      <c r="S405" s="3"/>
+      <c r="T405" s="3"/>
+      <c r="U405" s="3"/>
+    </row>
+    <row r="406" ht="45.0" customHeight="1">
+      <c r="A406" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B406" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C406" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="D406" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E406" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="F406" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G406" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H406" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I406" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J406" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K406" s="3"/>
+      <c r="L406" s="3"/>
+      <c r="M406" s="3"/>
+      <c r="N406" s="3"/>
+      <c r="O406" s="3"/>
+      <c r="P406" s="3"/>
+      <c r="Q406" s="3"/>
+      <c r="R406" s="3"/>
+      <c r="S406" s="3"/>
+      <c r="T406" s="3"/>
+      <c r="U406" s="3"/>
+    </row>
+    <row r="407" ht="45.0" customHeight="1">
+      <c r="A407" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="B407" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C407" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="D407" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E407" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="F407" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G407" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="H407" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I407" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J407" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K407" s="3"/>
+      <c r="L407" s="3"/>
+      <c r="M407" s="3"/>
+      <c r="N407" s="3"/>
+      <c r="O407" s="3"/>
+      <c r="P407" s="3"/>
+      <c r="Q407" s="3"/>
+      <c r="R407" s="3"/>
+      <c r="S407" s="3"/>
+      <c r="T407" s="3"/>
+      <c r="U407" s="3"/>
+    </row>
+    <row r="408" ht="45.0" customHeight="1">
+      <c r="A408" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B408" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C408" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D408" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E408" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F408" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G408" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H408" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I408" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J408" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K408" s="3"/>
+      <c r="L408" s="3"/>
+      <c r="M408" s="3"/>
+      <c r="N408" s="3"/>
+      <c r="O408" s="3"/>
+      <c r="P408" s="3"/>
+      <c r="Q408" s="3"/>
+      <c r="R408" s="3"/>
+      <c r="S408" s="3"/>
+      <c r="T408" s="3"/>
+      <c r="U408" s="3"/>
+    </row>
+    <row r="409" ht="45.0" customHeight="1">
+      <c r="A409" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B409" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="C409" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D409" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E409" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F409" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G409" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="H409" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I409" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J409" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K409" s="3"/>
+      <c r="L409" s="3"/>
+      <c r="M409" s="3"/>
+      <c r="N409" s="3"/>
+      <c r="O409" s="3"/>
+      <c r="P409" s="3"/>
+      <c r="Q409" s="3"/>
+      <c r="R409" s="3"/>
+      <c r="S409" s="3"/>
+      <c r="T409" s="3"/>
+      <c r="U409" s="3"/>
+    </row>
+    <row r="410" ht="45.0" customHeight="1">
+      <c r="A410" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B410" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="C410" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D410" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E410" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F410" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G410" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="H410" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I410" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J410" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K410" s="3"/>
+      <c r="L410" s="3"/>
+      <c r="M410" s="3"/>
+      <c r="N410" s="3"/>
+      <c r="O410" s="3"/>
+      <c r="P410" s="3"/>
+      <c r="Q410" s="3"/>
+      <c r="R410" s="3"/>
+      <c r="S410" s="3"/>
+      <c r="T410" s="3"/>
+      <c r="U410" s="3"/>
+    </row>
+    <row r="411" ht="45.0" customHeight="1">
+      <c r="A411" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B411" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C411" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D411" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E411" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F411" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G411" s="3" t="s">
+        <v>650</v>
+      </c>
+      <c r="H411" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I411" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J411" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K411" s="3"/>
+      <c r="L411" s="3"/>
+      <c r="M411" s="3"/>
+      <c r="N411" s="3"/>
+      <c r="O411" s="3"/>
+      <c r="P411" s="3"/>
+      <c r="Q411" s="3"/>
+      <c r="R411" s="3"/>
+      <c r="S411" s="3"/>
+      <c r="T411" s="3"/>
+      <c r="U411" s="3"/>
+    </row>
+    <row r="412" ht="45.0" customHeight="1">
+      <c r="A412" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B412" s="3" t="s">
+        <v>651</v>
+      </c>
+      <c r="C412" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D412" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E412" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F412" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G412" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="H412" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I412" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J412" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K412" s="3"/>
+      <c r="L412" s="3"/>
+      <c r="M412" s="3"/>
+      <c r="N412" s="3"/>
+      <c r="O412" s="3"/>
+      <c r="P412" s="3"/>
+      <c r="Q412" s="3"/>
+      <c r="R412" s="3"/>
+      <c r="S412" s="3"/>
+      <c r="T412" s="3"/>
+      <c r="U412" s="3"/>
+    </row>
+    <row r="413" ht="45.0" customHeight="1">
+      <c r="A413" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B413" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="C413" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D413" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E413" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F413" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G413" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="H413" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I413" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J413" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K413" s="3"/>
+      <c r="L413" s="3"/>
+      <c r="M413" s="3"/>
+      <c r="N413" s="3"/>
+      <c r="O413" s="3"/>
+      <c r="P413" s="3"/>
+      <c r="Q413" s="3"/>
+      <c r="R413" s="3"/>
+      <c r="S413" s="3"/>
+      <c r="T413" s="3"/>
+      <c r="U413" s="3"/>
+    </row>
+    <row r="414" ht="45.0" customHeight="1">
+      <c r="A414" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B414" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="C414" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D414" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E414" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F414" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G414" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="H414" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I414" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J414" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K414" s="3"/>
+      <c r="L414" s="3"/>
+      <c r="M414" s="3"/>
+      <c r="N414" s="3"/>
+      <c r="O414" s="3"/>
+      <c r="P414" s="3"/>
+      <c r="Q414" s="3"/>
+      <c r="R414" s="3"/>
+      <c r="S414" s="3"/>
+      <c r="T414" s="3"/>
+      <c r="U414" s="3"/>
+    </row>
+    <row r="415" ht="45.0" customHeight="1">
+      <c r="A415" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B415" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="C415" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D415" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E415" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F415" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G415" s="3" t="s">
+        <v>658</v>
+      </c>
+      <c r="H415" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I415" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J415" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K415" s="3"/>
+      <c r="L415" s="3"/>
+      <c r="M415" s="3"/>
+      <c r="N415" s="3"/>
+      <c r="O415" s="3"/>
+      <c r="P415" s="3"/>
+      <c r="Q415" s="3"/>
+      <c r="R415" s="3"/>
+      <c r="S415" s="3"/>
+      <c r="T415" s="3"/>
+      <c r="U415" s="3"/>
+    </row>
+    <row r="416" ht="45.0" customHeight="1">
+      <c r="A416" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B416" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="C416" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D416" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E416" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F416" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G416" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="H416" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I416" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J416" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K416" s="3"/>
+      <c r="L416" s="3"/>
+      <c r="M416" s="3"/>
+      <c r="N416" s="3"/>
+      <c r="O416" s="3"/>
+      <c r="P416" s="3"/>
+      <c r="Q416" s="3"/>
+      <c r="R416" s="3"/>
+      <c r="S416" s="3"/>
+      <c r="T416" s="3"/>
+      <c r="U416" s="3"/>
+    </row>
+    <row r="417" ht="45.0" customHeight="1">
+      <c r="A417" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B417" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="C417" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D417" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E417" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F417" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G417" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H417" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I417" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J417" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K417" s="3"/>
+      <c r="L417" s="3"/>
+      <c r="M417" s="3"/>
+      <c r="N417" s="3"/>
+      <c r="O417" s="3"/>
+      <c r="P417" s="3"/>
+      <c r="Q417" s="3"/>
+      <c r="R417" s="3"/>
+      <c r="S417" s="3"/>
+      <c r="T417" s="3"/>
+      <c r="U417" s="3"/>
+    </row>
+    <row r="418" ht="45.0" customHeight="1">
+      <c r="A418" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B418" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C418" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D418" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E418" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F418" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G418" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="H418" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="I418" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J418" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K418" s="3"/>
+      <c r="L418" s="3"/>
+      <c r="M418" s="3"/>
+      <c r="N418" s="3"/>
+      <c r="O418" s="3"/>
+      <c r="P418" s="3"/>
+      <c r="Q418" s="3"/>
+      <c r="R418" s="3"/>
+      <c r="S418" s="3"/>
+      <c r="T418" s="3"/>
+      <c r="U418" s="3"/>
+    </row>
+    <row r="419" ht="45.0" customHeight="1">
+      <c r="A419" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B419" s="3" t="s">
+        <v>664</v>
+      </c>
+      <c r="C419" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D419" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E419" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F419" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G419" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="H419" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I419" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J419" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K419" s="3"/>
+      <c r="L419" s="3"/>
+      <c r="M419" s="3"/>
+      <c r="N419" s="3"/>
+      <c r="O419" s="3"/>
+      <c r="P419" s="3"/>
+      <c r="Q419" s="3"/>
+      <c r="R419" s="3"/>
+      <c r="S419" s="3"/>
+      <c r="T419" s="3"/>
+      <c r="U419" s="3"/>
+    </row>
+    <row r="420" ht="45.0" customHeight="1">
+      <c r="A420" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B420" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="C420" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D420" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E420" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F420" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G420" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="H420" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I420" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J420" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K420" s="3"/>
+      <c r="L420" s="3"/>
+      <c r="M420" s="3"/>
+      <c r="N420" s="3"/>
+      <c r="O420" s="3"/>
+      <c r="P420" s="3"/>
+      <c r="Q420" s="3"/>
+      <c r="R420" s="3"/>
+      <c r="S420" s="3"/>
+      <c r="T420" s="3"/>
+      <c r="U420" s="3"/>
+    </row>
+    <row r="421" ht="45.0" customHeight="1">
+      <c r="A421" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B421" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="C421" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D421" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E421" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F421" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G421" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="H421" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I421" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J421" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K421" s="3"/>
+      <c r="L421" s="3"/>
+      <c r="M421" s="3"/>
+      <c r="N421" s="3"/>
+      <c r="O421" s="3"/>
+      <c r="P421" s="3"/>
+      <c r="Q421" s="3"/>
+      <c r="R421" s="3"/>
+      <c r="S421" s="3"/>
+      <c r="T421" s="3"/>
+      <c r="U421" s="3"/>
+    </row>
+    <row r="422" ht="45.0" customHeight="1">
+      <c r="A422" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="C422" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D422" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E422" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F422" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G422" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="H422" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I422" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J422" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K422" s="3"/>
+      <c r="L422" s="3"/>
+      <c r="M422" s="3"/>
+      <c r="N422" s="3"/>
+      <c r="O422" s="3"/>
+      <c r="P422" s="3"/>
+      <c r="Q422" s="3"/>
+      <c r="R422" s="3"/>
+      <c r="S422" s="3"/>
+      <c r="T422" s="3"/>
+      <c r="U422" s="3"/>
+    </row>
+    <row r="423" ht="45.0" customHeight="1">
+      <c r="A423" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="B423" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="C423" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D423" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E423" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F423" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G423" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H423" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I423" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J423" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K423" s="3"/>
+      <c r="L423" s="3"/>
+      <c r="M423" s="3"/>
+      <c r="N423" s="3"/>
+      <c r="O423" s="3"/>
+      <c r="P423" s="3"/>
+      <c r="Q423" s="3"/>
+      <c r="R423" s="3"/>
+      <c r="S423" s="3"/>
+      <c r="T423" s="3"/>
+      <c r="U423" s="3"/>
+    </row>
+    <row r="424" ht="45.0" customHeight="1">
+      <c r="A424" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="C424" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D424" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E424" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F424" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G424" s="17" t="s">
+        <v>674</v>
+      </c>
+      <c r="H424" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="I424" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J424" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K424" s="3"/>
+      <c r="L424" s="3"/>
+      <c r="M424" s="3"/>
+      <c r="N424" s="3"/>
+      <c r="O424" s="3"/>
+      <c r="P424" s="3"/>
+      <c r="Q424" s="3"/>
+      <c r="R424" s="3"/>
+      <c r="S424" s="3"/>
+      <c r="T424" s="3"/>
+      <c r="U424" s="3"/>
+    </row>
+    <row r="425" ht="45.0" customHeight="1">
+      <c r="A425" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B425" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="C425" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D425" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E425" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="F425" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G425" s="17" t="s">
+        <v>678</v>
+      </c>
+      <c r="H425" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I425" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J425" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K425" s="3"/>
+      <c r="L425" s="3"/>
+      <c r="M425" s="3"/>
+      <c r="N425" s="3"/>
+      <c r="O425" s="3"/>
+      <c r="P425" s="3"/>
+      <c r="Q425" s="3"/>
+      <c r="R425" s="3"/>
+      <c r="S425" s="3"/>
+      <c r="T425" s="3"/>
+      <c r="U425" s="3"/>
+    </row>
+    <row r="426" ht="45.0" customHeight="1">
+      <c r="A426" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B426" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="C426" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D426" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E426" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F426" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G426" s="17" t="s">
+        <v>680</v>
+      </c>
+      <c r="H426" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I426" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J426" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K426" s="3"/>
+      <c r="L426" s="3"/>
+      <c r="M426" s="3"/>
+      <c r="N426" s="3"/>
+      <c r="O426" s="3"/>
+      <c r="P426" s="3"/>
+      <c r="Q426" s="3"/>
+      <c r="R426" s="3"/>
+      <c r="S426" s="3"/>
+      <c r="T426" s="3"/>
+      <c r="U426" s="3"/>
+    </row>
+    <row r="427" ht="45.0" customHeight="1">
+      <c r="A427" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B427" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="C427" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D427" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E427" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F427" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G427" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="H427" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I427" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J427" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K427" s="3"/>
+      <c r="L427" s="3"/>
+      <c r="M427" s="3"/>
+      <c r="N427" s="3"/>
+      <c r="O427" s="3"/>
+      <c r="P427" s="3"/>
+      <c r="Q427" s="3"/>
+      <c r="R427" s="3"/>
+      <c r="S427" s="3"/>
+      <c r="T427" s="3"/>
+      <c r="U427" s="3"/>
+    </row>
+    <row r="428" ht="45.0" customHeight="1">
+      <c r="A428" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B428" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="C428" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D428" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E428" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="F428" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G428" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="H428" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I428" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J428" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K428" s="3"/>
+      <c r="L428" s="3"/>
+      <c r="M428" s="3"/>
+      <c r="N428" s="3"/>
+      <c r="O428" s="3"/>
+      <c r="P428" s="3"/>
+      <c r="Q428" s="3"/>
+      <c r="R428" s="3"/>
+      <c r="S428" s="3"/>
+      <c r="T428" s="3"/>
+      <c r="U428" s="3"/>
+    </row>
+    <row r="429" ht="45.0" customHeight="1">
+      <c r="A429" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B429" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="C429" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D429" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E429" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F429" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G429" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H429" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I429" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J429" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K429" s="3"/>
+      <c r="L429" s="3"/>
+      <c r="M429" s="3"/>
+      <c r="N429" s="3"/>
+      <c r="O429" s="3"/>
+      <c r="P429" s="3"/>
+      <c r="Q429" s="3"/>
+      <c r="R429" s="3"/>
+      <c r="S429" s="3"/>
+      <c r="T429" s="3"/>
+      <c r="U429" s="3"/>
+    </row>
+    <row r="430" ht="45.0" customHeight="1">
+      <c r="A430" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="B430" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="C430" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="D430" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E430" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F430" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G430" s="3" t="s">
+        <v>684</v>
+      </c>
+      <c r="H430" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I430" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J430" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K430" s="3"/>
+      <c r="L430" s="3"/>
+      <c r="M430" s="3"/>
+      <c r="N430" s="3"/>
+      <c r="O430" s="3"/>
+      <c r="P430" s="3"/>
+      <c r="Q430" s="3"/>
+      <c r="R430" s="3"/>
+      <c r="S430" s="3"/>
+      <c r="T430" s="3"/>
+      <c r="U430" s="3"/>
+    </row>
+    <row r="431" ht="45.0" customHeight="1">
+      <c r="A431" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B431" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="C431" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D431" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E431" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F431" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G431" s="3" t="s">
+        <v>687</v>
+      </c>
+      <c r="H431" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I431" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J431" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K431" s="3"/>
+      <c r="L431" s="3"/>
+      <c r="M431" s="3"/>
+      <c r="N431" s="3"/>
+      <c r="O431" s="3"/>
+      <c r="P431" s="3"/>
+      <c r="Q431" s="3"/>
+      <c r="R431" s="3"/>
+      <c r="S431" s="3"/>
+      <c r="T431" s="3"/>
+      <c r="U431" s="3"/>
+    </row>
+    <row r="432" ht="45.0" customHeight="1">
+      <c r="A432" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B432" s="3" t="s">
+        <v>688</v>
+      </c>
+      <c r="C432" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D432" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E432" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F432" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G432" s="3" t="s">
+        <v>689</v>
+      </c>
+      <c r="H432" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I432" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J432" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K432" s="3"/>
+      <c r="L432" s="3"/>
+      <c r="M432" s="3"/>
+      <c r="N432" s="3"/>
+      <c r="O432" s="3"/>
+      <c r="P432" s="3"/>
+      <c r="Q432" s="3"/>
+      <c r="R432" s="3"/>
+      <c r="S432" s="3"/>
+      <c r="T432" s="3"/>
+      <c r="U432" s="3"/>
+    </row>
+    <row r="433" ht="45.0" customHeight="1">
+      <c r="A433" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B433" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="C433" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D433" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E433" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F433" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G433" s="3" t="s">
+        <v>691</v>
+      </c>
+      <c r="H433" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I433" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J433" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K433" s="3"/>
+      <c r="L433" s="3"/>
+      <c r="M433" s="3"/>
+      <c r="N433" s="3"/>
+      <c r="O433" s="3"/>
+      <c r="P433" s="3"/>
+      <c r="Q433" s="3"/>
+      <c r="R433" s="3"/>
+      <c r="S433" s="3"/>
+      <c r="T433" s="3"/>
+      <c r="U433" s="3"/>
+    </row>
+    <row r="434" ht="45.0" customHeight="1">
+      <c r="A434" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B434" s="3" t="s">
+        <v>692</v>
+      </c>
+      <c r="C434" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D434" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E434" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F434" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G434" s="3" t="s">
+        <v>693</v>
+      </c>
+      <c r="H434" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I434" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J434" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K434" s="3"/>
+      <c r="L434" s="3"/>
+      <c r="M434" s="3"/>
+      <c r="N434" s="3"/>
+      <c r="O434" s="3"/>
+      <c r="P434" s="3"/>
+      <c r="Q434" s="3"/>
+      <c r="R434" s="3"/>
+      <c r="S434" s="3"/>
+      <c r="T434" s="3"/>
+      <c r="U434" s="3"/>
+    </row>
+    <row r="435" ht="45.0" customHeight="1">
+      <c r="A435" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B435" s="3" t="s">
+        <v>694</v>
+      </c>
+      <c r="C435" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D435" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E435" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F435" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G435" s="3" t="s">
+        <v>695</v>
+      </c>
+      <c r="H435" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I435" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J435" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K435" s="3"/>
+      <c r="L435" s="3"/>
+      <c r="M435" s="3"/>
+      <c r="N435" s="3"/>
+      <c r="O435" s="3"/>
+      <c r="P435" s="3"/>
+      <c r="Q435" s="3"/>
+      <c r="R435" s="3"/>
+      <c r="S435" s="3"/>
+      <c r="T435" s="3"/>
+      <c r="U435" s="3"/>
+    </row>
+    <row r="436" ht="45.0" customHeight="1">
+      <c r="A436" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="B436" s="3" t="s">
+        <v>696</v>
+      </c>
+      <c r="C436" s="3" t="s">
+        <v>685</v>
+      </c>
+      <c r="D436" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E436" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F436" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G436" s="3" t="s">
+        <v>697</v>
+      </c>
+      <c r="H436" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I436" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J436" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K436" s="3"/>
+      <c r="L436" s="3"/>
+      <c r="M436" s="3"/>
+      <c r="N436" s="3"/>
+      <c r="O436" s="3"/>
+      <c r="P436" s="3"/>
+      <c r="Q436" s="3"/>
+      <c r="R436" s="3"/>
+      <c r="S436" s="3"/>
+      <c r="T436" s="3"/>
+      <c r="U436" s="3"/>
+    </row>
+    <row r="437" ht="45.0" customHeight="1">
+      <c r="A437" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>699</v>
+      </c>
+      <c r="C437" s="3" t="s">
+        <v>698</v>
+      </c>
+      <c r="D437" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E437" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F437" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G437" s="3" t="s">
+        <v>700</v>
+      </c>
+      <c r="H437" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I437" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J437" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K437" s="3"/>
+      <c r="L437" s="3"/>
+      <c r="M437" s="3"/>
+      <c r="N437" s="3"/>
+      <c r="O437" s="3"/>
+      <c r="P437" s="3"/>
+      <c r="Q437" s="3"/>
+      <c r="R437" s="3"/>
+      <c r="S437" s="3"/>
+      <c r="T437" s="3"/>
+      <c r="U437" s="3"/>
+    </row>
     <row r="438" ht="45.0" customHeight="1"/>
     <row r="439" ht="45.0" customHeight="1"/>
     <row r="440" ht="45.0" customHeight="1"/>

</xml_diff>

<commit_message>
Adding 18 more cases to maven demo
</commit_message>
<xml_diff>
--- a/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
+++ b/src/test/resources/auto-test-resources/maven-demo-integration-resources.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4078" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4138" uniqueCount="711">
   <si>
     <t>Class</t>
   </si>
@@ -2529,6 +2529,46 @@
   </si>
   <si>
     <t>Good Day</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.resttemplate.PostController</t>
+  </si>
+  <si>
+    <t>getAllPosts
+()Ljava/util/List&lt;Lorg/unlogged/demo/resttemplate/Post;&gt;;</t>
+  </si>
+  <si>
+    <t>[{"userId":1,"id":1,"title":"sunt aut facere repellat provident occaecati excepturi optio reprehenderit","body":"quia et suscipit\nsuscipit recusandae consequuntur expedita et cum\nreprehenderit molestiae ut ut quas totam\nnostrum rerum est autem sunt rem eveniet architecto"},{"userId":1,"id":2,"title":"qui est esse","body":"est rerum tempore vitae\nsequi sint nihil reprehenderit dolor beatae ea dolores neque\nfugiat blanditiis voluptate porro vel nihil molestiae ut reiciendis\nqui aperiam non debitis possimus qui neque nisi nulla"},{"userId":1,"id":3,"title":"ea molestias quasi exercitationem repellat qui ipsa sit aut","body":"et iusto sed quo iure\nvoluptatem occaecati omnis eligendi aut ad\nvoluptatem doloribus vel accusantium quis pariatur\nmolestiae porro eius odio et labore et velit aut"},{"userId":1,"id":4,"title":"eum et est occaecati","body":"ullam et saepe reiciendis voluptatem adipisci\nsit amet autem assumenda provident rerum culpa\nquis hic commodi nesciunt rem tenetur doloremque ipsam iure\nquis sunt voluptatem rerum illo velit"},{"userId":1,"id":5,"title":"nesciunt quas odio","body":"repudiandae veniam quaerat sunt sed\nalias aut fugiat sit autem sed est\nvoluptatem omnis possimus esse voluptatibus quis\nest aut tenetur dolor neque"},{"userId":1,"id":6,"title":"dolorem eum magni eos aperiam quia","body":"ut aspernatur corporis harum nihil quis provident sequi\nmollitia nobis aliquid molestiae\nperspiciatis et ea nemo ab reprehenderit accusantium quas\nvoluptate dolores velit et doloremque molestiae"},{"userId":1,"id":7,"title":"magnam facilis autem","body":"dolore placeat quibusdam ea quo vitae\nmagni quis enim qui quis quo nemo aut saepe\nquidem repellat excepturi ut quia\nsunt ut sequi eos ea sed quas"},{"userId":1,"id":8,"title":"dolorem dolore est ipsam","body":"dignissimos aperiam dolorem qui eum\nfacilis quibusdam animi sint suscipit qui sint possimus cum\nquaerat magni maiores excepturi\nipsam ut commodi dolor voluptatum modi aut vitae"},{"userId":1,"id":9,"title":"nesciunt iure omnis dolorem tempora et accusantium","body":"consectetur animi nesciunt iure dolore\nenim quia ad\nveniam autem ut quam aut nobis\net est aut quod aut provident voluptas autem voluptas"},{"userId":1,"id":10,"title":"optio molestias id quia eum","body":"quo et expedita modi cum officia vel magni\ndoloribus qui repudiandae\nvero nisi sit\nquos veniam quod sed accusamus veritatis error"},{"userId":2,"id":11,"title":"et ea vero quia laudantium autem","body":"delectus reiciendis molestiae occaecati non minima eveniet qui voluptatibus\naccusamus in eum beatae sit\nvel qui neque voluptates ut commodi qui incidunt\nut animi commodi"},{"userId":2,"id":12,"title":"in quibusdam tempore odit est dolorem","body":"itaque id aut magnam\npraesentium quia et ea odit et ea voluptas et\nsapiente quia nihil amet occaecati quia id voluptatem\nincidunt ea est distinctio odio"},{"userId":2,"id":13,"title":"dolorum ut in voluptas mollitia et saepe quo animi","body":"aut dicta possimus sint mollitia voluptas commodi quo doloremque\niste corrupti reiciendis voluptatem eius rerum\nsit cumque quod eligendi laborum minima\nperferendis recusandae assumenda consectetur porro architecto ipsum ipsam"},{"userId":2,"id":14,"title":"voluptatem eligendi optio","body":"fuga et accusamus dolorum perferendis illo voluptas\nnon doloremque neque facere\nad qui dolorum molestiae beatae\nsed aut voluptas totam sit illum"},{"userId":2,"id":15,"title":"eveniet quod temporibus","body":"reprehenderit quos placeat\nvelit minima officia dolores impedit repudiandae molestiae nam\nvoluptas recusandae quis delectus\nofficiis harum fugiat vitae"},{"userId":2,"id":16,"title":"sint suscipit perspiciatis velit dolorum rerum ipsa laboriosam odio","body":"suscipit nam nisi quo aperiam aut\nasperiores eos fugit maiores voluptatibus quia\nvoluptatem quis ullam qui in alias quia est\nconsequatur magni mollitia accusamus ea nisi voluptate dicta"},{"userId":2,"id":17,"title":"fugit voluptas sed molestias voluptatem provident","body":"eos voluptas et aut odit natus earum\naspernatur fuga molestiae ullam\ndeserunt ratione qui eos\nqui nihil ratione nemo velit ut aut id quo"},{"userId":2,"id":18,"title":"voluptate et itaque vero tempora molestiae","body":"eveniet quo quis\nlaborum totam consequatur non dolor\nut et est repudiandae\nest voluptatem vel debitis et magnam"},{"userId":2,"id":19,"title":"adipisci placeat illum aut reiciendis qui","body":"illum quis cupiditate provident sit magnam\nea sed aut omnis\nveniam maiores ullam consequatur atque\nadipisci quo iste expedita sit quos voluptas"},{"userId":2,"id":20,"title":"doloribus ad provident suscipit at","body":"qui consequuntur ducimus possimus quisquam amet similique\nsuscipit porro ipsam amet\neos veritatis officiis exercitationem vel fugit aut necessitatibus totam\nomnis rerum consequatur expedita quidem cumque explicabo"},{"userId":3,"id":21,"title":"asperiores ea ipsam voluptatibus modi minima quia sint","body":"repellat aliquid praesentium dolorem quo\nsed totam minus non itaque\nnihil labore molestiae sunt dolor eveniet hic recusandae veniam\ntempora et tenetur expedita sunt"},{"userId":3,"id":22,"title":"dolor sint quo a velit explicabo quia nam","body":"eos qui et ipsum ipsam suscipit aut\nsed omnis non odio\nexpedita earum mollitia molestiae aut atque rem suscipit\nnam impedit esse"},{"userId":3,"id":23,"title":"maxime id vitae nihil numquam","body":"veritatis unde neque eligendi\nquae quod architecto quo neque vitae\nest illo sit tempora doloremque fugit quod\net et vel beatae sequi ullam sed tenetur perspiciatis"},{"userId":3,"id":24,"title":"autem hic labore sunt dolores incidunt","body":"enim et ex nulla\nomnis voluptas quia qui\nvoluptatem consequatur numquam aliquam sunt\ntotam recusandae id dignissimos aut sed asperiores deserunt"},{"userId":3,"id":25,"title":"rem alias distinctio quo quis","body":"ullam consequatur ut\nomnis quis sit vel consequuntur\nipsa eligendi ipsum molestiae et omnis error nostrum\nmolestiae illo tempore quia et distinctio"},{"userId":3,"id":26,"title":"est et quae odit qui non","body":"similique esse doloribus nihil accusamus\nomnis dolorem fuga consequuntur reprehenderit fugit recusandae temporibus\nperspiciatis cum ut laudantium\nomnis aut molestiae vel vero"},{"userId":3,"id":27,"title":"quasi id et eos tenetur aut quo autem","body":"eum sed dolores ipsam sint possimus debitis occaecati\ndebitis qui qui et\nut placeat enim earum aut odit facilis\nconsequatur suscipit necessitatibus rerum sed inventore temporibus consequatur"},{"userId":3,"id":28,"title":"delectus ullam et corporis nulla voluptas sequi","body":"non et quaerat ex quae ad maiores\nmaiores recusandae totam aut blanditiis mollitia quas illo\nut voluptatibus voluptatem\nsimilique nostrum eum"},{"userId":3,"id":29,"title":"iusto eius quod necessitatibus culpa ea","body":"odit magnam ut saepe sed non qui\ntempora atque nihil\naccusamus illum doloribus illo dolor\neligendi repudiandae odit magni similique sed cum maiores"},{"userId":3,"id":30,"title":"a quo magni similique perferendis","body":"alias dolor cumque\nimpedit blanditiis non eveniet odio maxime\nblanditiis amet eius quis tempora quia autem rem\na provident perspiciatis quia"},{"userId":4,"id":31,"title":"ullam ut quidem id aut vel consequuntur","body":"debitis eius sed quibusdam non quis consectetur vitae\nimpedit ut qui consequatur sed aut in\nquidem sit nostrum et maiores adipisci atque\nquaerat voluptatem adipisci repudiandae"},{"userId":4,"id":32,"title":"doloremque illum aliquid sunt","body":"deserunt eos nobis asperiores et hic\nest debitis repellat molestiae optio\nnihil ratione ut eos beatae quibusdam distinctio maiores\nearum voluptates et aut adipisci ea maiores voluptas maxime"},{"userId":4,"id":33,"title":"qui explicabo molestiae dolorem","body":"rerum ut et numquam laborum odit est sit\nid qui sint in\nquasi tenetur tempore aperiam et quaerat qui in\nrerum officiis sequi cumque quod"},{"userId":4,"id":34,"title":"magnam ut rerum iure","body":"ea velit perferendis earum ut voluptatem voluptate itaque iusto\ntotam pariatur in\nnemo voluptatem voluptatem autem magni tempora minima in\nest distinctio qui assumenda accusamus dignissimos officia nesciunt nobis"},{"userId":4,"id":35,"title":"id nihil consequatur molestias animi provident","body":"nisi error delectus possimus ut eligendi vitae\nplaceat eos harum cupiditate facilis reprehenderit voluptatem beatae\nmodi ducimus quo illum voluptas eligendi\net nobis quia fugit"},{"userId":4,"id":36,"title":"fuga nam accusamus voluptas reiciendis itaque","body":"ad mollitia et omnis minus architecto odit\nvoluptas doloremque maxime aut non ipsa qui alias veniam\nblanditiis culpa aut quia nihil cumque facere et occaecati\nqui aspernatur quia eaque ut aperiam inventore"},{"userId":4,"id":37,"title":"provident vel ut sit ratione est","body":"debitis et eaque non officia sed nesciunt pariatur vel\nvoluptatem iste vero et ea\nnumquam aut expedita ipsum nulla in\nvoluptates omnis consequatur aut enim officiis in quam qui"},{"userId":4,"id":38,"title":"explicabo et eos deleniti nostrum ab id repellendus","body":"animi esse sit aut sit nesciunt assumenda eum voluptas\nquia voluptatibus provident quia necessitatibus ea\nrerum repudiandae quia voluptatem delectus fugit aut id quia\nratione optio eos iusto veniam iure"},{"userId":4,"id":39,"title":"eos dolorem iste accusantium est eaque quam","body":"corporis rerum ducimus vel eum accusantium\nmaxime aspernatur a porro possimus iste omnis\nest in deleniti asperiores fuga aut\nvoluptas sapiente vel dolore minus voluptatem incidunt ex"},{"userId":4,"id":40,"title":"enim quo cumque","body":"ut voluptatum aliquid illo tenetur nemo sequi quo facilis\nipsum rem optio mollitia quas\nvoluptatem eum voluptas qui\nunde omnis voluptatem iure quasi maxime voluptas nam"},{"userId":5,"id":41,"title":"non est facere","body":"molestias id nostrum\nexcepturi molestiae dolore omnis repellendus quaerat saepe\nconsectetur iste quaerat tenetur asperiores accusamus ex ut\nnam quidem est ducimus sunt debitis saepe"},{"userId":5,"id":42,"title":"commodi ullam sint et excepturi error explicabo praesentium voluptas","body":"odio fugit voluptatum ducimus earum autem est incidunt voluptatem\nodit reiciendis aliquam sunt sequi nulla dolorem\nnon facere repellendus voluptates quia\nratione harum vitae ut"},{"userId":5,"id":43,"title":"eligendi iste nostrum consequuntur adipisci praesentium sit beatae perferendis","body":"similique fugit est\nillum et dolorum harum et voluptate eaque quidem\nexercitationem quos nam commodi possimus cum odio nihil nulla\ndolorum exercitationem magnam ex et a et distinctio debitis"},{"userId":5,"id":44,"title":"optio dolor molestias sit","body":"temporibus est consectetur dolore\net libero debitis vel velit laboriosam quia\nipsum quibusdam qui itaque fuga rem aut\nea et iure quam sed maxime ut distinctio quae"},{"userId":5,"id":45,"title":"ut numquam possimus omnis eius suscipit laudantium iure","body":"est natus reiciendis nihil possimus aut provident\nex et dolor\nrepellat pariatur est\nnobis rerum repellendus dolorem autem"},{"userId":5,"id":46,"title":"aut quo modi neque nostrum ducimus","body":"voluptatem quisquam iste\nvoluptatibus natus officiis facilis dolorem\nquis quas ipsam\nvel et voluptatum in aliquid"},{"userId":5,"id":47,"title":"quibusdam cumque rem aut deserunt","body":"voluptatem assumenda ut qui ut cupiditate aut impedit veniam\noccaecati nemo illum voluptatem laudantium\nmolestiae beatae rerum ea iure soluta nostrum\neligendi et voluptate"},{"userId":5,"id":48,"title":"ut voluptatem illum ea doloribus itaque eos","body":"voluptates quo voluptatem facilis iure occaecati\nvel assumenda rerum officia et\nillum perspiciatis ab deleniti\nlaudantium repellat ad ut et autem reprehenderit"},{"userId":5,"id":49,"title":"laborum non sunt aut ut assumenda perspiciatis voluptas","body":"inventore ab sint\nnatus fugit id nulla sequi architecto nihil quaerat\neos tenetur in in eum veritatis non\nquibusdam officiis aspernatur cumque aut commodi aut"},{"userId":5,"id":50,"title":"repellendus qui recusandae incidunt voluptates tenetur qui omnis exercitationem","body":"error suscipit maxime adipisci consequuntur recusandae\nvoluptas eligendi et est et voluptates\nquia distinctio ab amet quaerat molestiae et vitae\nadipisci impedit sequi nesciunt quis consectetur"},{"userId":6,"id":51,"title":"soluta aliquam aperiam consequatur illo quis voluptas","body":"sunt dolores aut doloribus\ndolore doloribus voluptates tempora et\ndoloremque et quo\ncum asperiores sit consectetur dolorem"},{"userId":6,"id":52,"title":"qui enim et consequuntur quia animi quis voluptate quibusdam","body":"iusto est quibusdam fuga quas quaerat molestias\na enim ut sit accusamus enim\ntemporibus iusto accusantium provident architecto\nsoluta esse reprehenderit qui laborum"},{"userId":6,"id":53,"title":"ut quo aut ducimus alias","body":"minima harum praesentium eum rerum illo dolore\nquasi exercitationem rerum nam\nporro quis neque quo\nconsequatur minus dolor quidem veritatis sunt non explicabo similique"},{"userId":6,"id":54,"title":"sit asperiores ipsam eveniet odio non quia","body":"totam corporis dignissimos\nvitae dolorem ut occaecati accusamus\nex velit deserunt\net exercitationem vero incidunt corrupti mollitia"},{"userId":6,"id":55,"title":"sit vel voluptatem et non libero","body":"debitis excepturi ea perferendis harum libero optio\neos accusamus cum fuga ut sapiente repudiandae\net ut incidunt omnis molestiae\nnihil ut eum odit"},{"userId":6,"id":56,"title":"qui et at rerum necessitatibus","body":"aut est omnis dolores\nneque rerum quod ea rerum velit pariatur beatae excepturi\net provident voluptas corrupti\ncorporis harum reprehenderit dolores eligendi"},{"userId":6,"id":57,"title":"sed ab est est","body":"at pariatur consequuntur earum quidem\nquo est laudantium soluta voluptatem\nqui ullam et est\net cum voluptas voluptatum repellat est"},{"userId":6,"id":58,"title":"voluptatum itaque dolores nisi et quasi","body":"veniam voluptatum quae adipisci id\net id quia eos ad et dolorem\naliquam quo nisi sunt eos impedit error\nad similique veniam"},{"userId":6,"id":59,"title":"qui commodi dolor at maiores et quis id accusantium","body":"perspiciatis et quam ea autem temporibus non voluptatibus qui\nbeatae a earum officia nesciunt dolores suscipit voluptas et\nanimi doloribus cum rerum quas et magni\net hic ut ut commodi expedita sunt"},{"userId":6,"id":60,"title":"consequatur placeat omnis quisquam quia reprehenderit fugit veritatis facere","body":"asperiores sunt ab assumenda cumque modi velit\nqui esse omnis\nvoluptate et fuga perferendis voluptas\nillo ratione amet aut et omnis"},{"userId":7,"id":61,"title":"voluptatem doloribus consectetur est ut ducimus","body":"ab nemo optio odio\ndelectus tenetur corporis similique nobis repellendus rerum omnis facilis\nvero blanditiis debitis in nesciunt doloribus dicta dolores\nmagnam minus velit"},{"userId":7,"id":62,"title":"beatae enim quia vel","body":"enim aspernatur illo distinctio quae praesentium\nbeatae alias amet delectus qui voluptate distinctio\nodit sint accusantium autem omnis\nquo molestiae omnis ea eveniet optio"},{"userId":7,"id":63,"title":"voluptas blanditiis repellendus animi ducimus error sapiente et suscipit","body":"enim adipisci aspernatur nemo\nnumquam omnis facere dolorem dolor ex quis temporibus incidunt\nab delectus culpa quo reprehenderit blanditiis asperiores\naccusantium ut quam in voluptatibus voluptas ipsam dicta"},{"userId":7,"id":64,"title":"et fugit quas eum in in aperiam quod","body":"id velit blanditiis\neum ea voluptatem\nmolestiae sint occaecati est eos perspiciatis\nincidunt a error provident eaque aut aut qui"},{"userId":7,"id":65,"title":"consequatur id enim sunt et et","body":"voluptatibus ex esse\nsint explicabo est aliquid cumque adipisci fuga repellat labore\nmolestiae corrupti ex saepe at asperiores et perferendis\nnatus id esse incidunt pariatur"},{"userId":7,"id":66,"title":"repudiandae ea animi iusto","body":"officia veritatis tenetur vero qui itaque\nsint non ratione\nsed et ut asperiores iusto eos molestiae nostrum\nveritatis quibusdam et nemo iusto saepe"},{"userId":7,"id":67,"title":"aliquid eos sed fuga est maxime repellendus","body":"reprehenderit id nostrum\nvoluptas doloremque pariatur sint et accusantium quia quod aspernatur\net fugiat amet\nnon sapiente et consequatur necessitatibus molestiae"},{"userId":7,"id":68,"title":"odio quis facere architecto reiciendis optio","body":"magnam molestiae perferendis quisquam\nqui cum reiciendis\nquaerat animi amet hic inventore\nea quia deleniti quidem saepe porro velit"},{"userId":7,"id":69,"title":"fugiat quod pariatur odit minima","body":"officiis error culpa consequatur modi asperiores et\ndolorum assumenda voluptas et vel qui aut vel rerum\nvoluptatum quisquam perspiciatis quia rerum consequatur totam quas\nsequi commodi repudiandae asperiores et saepe a"},{"userId":7,"id":70,"title":"voluptatem laborum magni","body":"sunt repellendus quae\nest asperiores aut deleniti esse accusamus repellendus quia aut\nquia dolorem unde\neum tempora esse dolore"},{"userId":8,"id":71,"title":"et iusto veniam et illum aut fuga","body":"occaecati a doloribus\niste saepe consectetur placeat eum voluptate dolorem et\nqui quo quia voluptas\nrerum ut id enim velit est perferendis"},{"userId":8,"id":72,"title":"sint hic doloribus consequatur eos non id","body":"quam occaecati qui deleniti consectetur\nconsequatur aut facere quas exercitationem aliquam hic voluptas\nneque id sunt ut aut accusamus\nsunt consectetur expedita inventore velit"},{"userId":8,"id":73,"title":"consequuntur deleniti eos quia temporibus ab aliquid at","body":"voluptatem cumque tenetur consequatur expedita ipsum nemo quia explicabo\naut eum minima consequatur\ntempore cumque quae est et\net in consequuntur voluptatem voluptates aut"},{"userId":8,"id":74,"title":"enim unde ratione doloribus quas enim ut sit sapiente","body":"odit qui et et necessitatibus sint veniam\nmollitia amet doloremque molestiae commodi similique magnam et quam\nblanditiis est itaque\nquo et tenetur ratione occaecati molestiae tempora"},{"userId":8,"id":75,"title":"dignissimos eum dolor ut enim et delectus in","body":"commodi non non omnis et voluptas sit\nautem aut nobis magnam et sapiente voluptatem\net laborum repellat qui delectus facilis temporibus\nrerum amet et nemo voluptate expedita adipisci error dolorem"},{"userId":8,"id":76,"title":"doloremque officiis ad et non perferendis","body":"ut animi facere\ntotam iusto tempore\nmolestiae eum aut et dolorem aperiam\nquaerat recusandae totam odio"},{"userId":8,"id":77,"title":"necessitatibus quasi exercitationem odio","body":"modi ut in nulla repudiandae dolorum nostrum eos\naut consequatur omnis\nut incidunt est omnis iste et quam\nvoluptates sapiente aliquam asperiores nobis amet corrupti repudiandae provident"},{"userId":8,"id":78,"title":"quam voluptatibus rerum veritatis","body":"nobis facilis odit tempore cupiditate quia\nassumenda doloribus rerum qui ea\nillum et qui totam\naut veniam repellendus"},{"userId":8,"id":79,"title":"pariatur consequatur quia magnam autem omnis non amet","body":"libero accusantium et et facere incidunt sit dolorem\nnon excepturi qui quia sed laudantium\nquisquam molestiae ducimus est\nofficiis esse molestiae iste et quos"},{"userId":8,"id":80,"title":"labore in ex et explicabo corporis aut quas","body":"ex quod dolorem ea eum iure qui provident amet\nquia qui facere excepturi et repudiandae\nasperiores molestias provident\nminus incidunt vero fugit rerum sint sunt excepturi provident"},{"userId":9,"id":81,"title":"tempora rem veritatis voluptas quo dolores vero","body":"facere qui nesciunt est voluptatum voluptatem nisi\nsequi eligendi necessitatibus ea at rerum itaque\nharum non ratione velit laboriosam quis consequuntur\nex officiis minima doloremque voluptas ut aut"},{"userId":9,"id":82,"title":"laudantium voluptate suscipit sunt enim enim","body":"ut libero sit aut totam inventore sunt\nporro sint qui sunt molestiae\nconsequatur cupiditate qui iste ducimus adipisci\ndolor enim assumenda soluta laboriosam amet iste delectus hic"},{"userId":9,"id":83,"title":"odit et voluptates doloribus alias odio et","body":"est molestiae facilis quis tempora numquam nihil qui\nvoluptate sapiente consequatur est qui\nnecessitatibus autem aut ipsa aperiam modi dolore numquam\nreprehenderit eius rem quibusdam"},{"userId":9,"id":84,"title":"optio ipsam molestias necessitatibus occaecati facilis veritatis dolores aut","body":"sint molestiae magni a et quos\neaque et quasi\nut rerum debitis similique veniam\nrecusandae dignissimos dolor incidunt consequatur odio"},{"userId":9,"id":85,"title":"dolore veritatis porro provident adipisci blanditiis et sunt","body":"similique sed nisi voluptas iusto omnis\nmollitia et quo\nassumenda suscipit officia magnam sint sed tempora\nenim provident pariatur praesentium atque animi amet ratione"},{"userId":9,"id":86,"title":"placeat quia et porro iste","body":"quasi excepturi consequatur iste autem temporibus sed molestiae beatae\net quaerat et esse ut\nvoluptatem occaecati et vel explicabo autem\nasperiores pariatur deserunt optio"},{"userId":9,"id":87,"title":"nostrum quis quasi placeat","body":"eos et molestiae\nnesciunt ut a\ndolores perspiciatis repellendus repellat aliquid\nmagnam sint rem ipsum est"},{"userId":9,"id":88,"title":"sapiente omnis fugit eos","body":"consequatur omnis est praesentium\nducimus non iste\nneque hic deserunt\nvoluptatibus veniam cum et rerum sed"},{"userId":9,"id":89,"title":"sint soluta et vel magnam aut ut sed qui","body":"repellat aut aperiam totam temporibus autem et\narchitecto magnam ut\nconsequatur qui cupiditate rerum quia soluta dignissimos nihil iure\ntempore quas est"},{"userId":9,"id":90,"title":"ad iusto omnis odit dolor voluptatibus","body":"minus omnis soluta quia\nqui sed adipisci voluptates illum ipsam voluptatem\neligendi officia ut in\neos soluta similique molestias praesentium blanditiis"},{"userId":10,"id":91,"title":"aut amet sed","body":"libero voluptate eveniet aperiam sed\nsunt placeat suscipit molestias\nsimilique fugit nam natus\nexpedita consequatur consequatur dolores quia eos et placeat"},{"userId":10,"id":92,"title":"ratione ex tenetur perferendis","body":"aut et excepturi dicta laudantium sint rerum nihil\nlaudantium et at\na neque minima officia et similique libero et\ncommodi voluptate qui"},{"userId":10,"id":93,"title":"beatae soluta recusandae","body":"dolorem quibusdam ducimus consequuntur dicta aut quo laboriosam\nvoluptatem quis enim recusandae ut sed sunt\nnostrum est odit totam\nsit error sed sunt eveniet provident qui nulla"},{"userId":10,"id":94,"title":"qui qui voluptates illo iste minima","body":"aspernatur expedita soluta quo ab ut similique\nexpedita dolores amet\nsed temporibus distinctio magnam saepe deleniti\nomnis facilis nam ipsum natus sint similique omnis"},{"userId":10,"id":95,"title":"id minus libero illum nam ad officiis","body":"earum voluptatem facere provident blanditiis velit laboriosam\npariatur accusamus odio saepe\ncumque dolor qui a dicta ab doloribus consequatur omnis\ncorporis cupiditate eaque assumenda ad nesciunt"},{"userId":10,"id":96,"title":"quaerat velit veniam amet cupiditate aut numquam ut sequi","body":"in non odio excepturi sint eum\nlabore voluptates vitae quia qui et\ninventore itaque rerum\nveniam non exercitationem delectus aut"},{"userId":10,"id":97,"title":"quas fugiat ut perspiciatis vero provident","body":"eum non blanditiis soluta porro quibusdam voluptas\nvel voluptatem qui placeat dolores qui velit aut\nvel inventore aut cumque culpa explicabo aliquid at\nperspiciatis est et voluptatem dignissimos dolor itaque sit nam"},{"userId":10,"id":98,"title":"laboriosam dolor voluptates","body":"doloremque ex facilis sit sint culpa\nsoluta assumenda eligendi non ut eius\nsequi ducimus vel quasi\nveritatis est dolores"},{"userId":10,"id":99,"title":"temporibus sit alias delectus eligendi possimus magni","body":"quo deleniti praesentium dicta non quod\naut est molestias\nmolestias et officia quis nihil\nitaque dolorem quia"},{"userId":10,"id":100,"title":"at nam consequatur ea labore ea harum","body":"cupiditate quo est a modi nesciunt soluta\nipsa voluptas error itaque dicta in\nautem qui minus magnam et distinctio eum\naccusamus ratione error aut"}]</t>
+  </si>
+  <si>
+    <t>getPostById
+(I)Ljava/lang/String;</t>
+  </si>
+  <si>
+    <t>Exception: Failed to fetch post with id 0</t>
+  </si>
+  <si>
+    <t>[int : "1"
+]</t>
+  </si>
+  <si>
+    <t>{
+  "userId": 1,
+  "id": 1,
+  "title": "sunt aut facere repellat provident occaecati excepturi optio reprehenderit",
+  "body": "quia et suscipit\nsuscipit recusandae consequuntur expedita et cum\nreprehenderit molestiae ut ut quas totam\nnostrum rerum est autem sunt rem eveniet architecto"
+}</t>
+  </si>
+  <si>
+    <t>org.unlogged.demo.resttemplate.PostsClient</t>
+  </si>
+  <si>
+    <t>findAll
+()Ljava/util/List&lt;Lorg/unlogged/demo/resttemplate/Post;&gt;;</t>
+  </si>
+  <si>
+    <t>findById
+(I)Ljava/lang/String;</t>
   </si>
 </sst>
 </file>
@@ -2586,7 +2626,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2638,6 +2678,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -17393,12 +17436,270 @@
       <c r="T437" s="3"/>
       <c r="U437" s="3"/>
     </row>
-    <row r="438" ht="45.0" customHeight="1"/>
-    <row r="439" ht="45.0" customHeight="1"/>
-    <row r="440" ht="45.0" customHeight="1"/>
-    <row r="441" ht="45.0" customHeight="1"/>
-    <row r="442" ht="45.0" customHeight="1"/>
-    <row r="443" ht="45.0" customHeight="1"/>
+    <row r="438" ht="45.0" customHeight="1">
+      <c r="A438" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>702</v>
+      </c>
+      <c r="C438" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D438" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E438" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F438" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G438" s="18" t="s">
+        <v>703</v>
+      </c>
+      <c r="H438" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I438" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J438" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K438" s="3"/>
+      <c r="L438" s="3"/>
+      <c r="M438" s="3"/>
+      <c r="N438" s="3"/>
+      <c r="O438" s="3"/>
+      <c r="P438" s="3"/>
+      <c r="Q438" s="3"/>
+      <c r="R438" s="3"/>
+      <c r="S438" s="3"/>
+      <c r="T438" s="3"/>
+      <c r="U438" s="3"/>
+      <c r="V438" s="3"/>
+    </row>
+    <row r="439" ht="45.0" customHeight="1">
+      <c r="A439" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B439" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C439" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D439" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E439" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F439" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G439" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="H439" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="I439" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J439" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K439" s="3"/>
+      <c r="L439" s="3"/>
+      <c r="M439" s="3"/>
+      <c r="N439" s="3"/>
+      <c r="O439" s="3"/>
+      <c r="P439" s="3"/>
+      <c r="Q439" s="3"/>
+      <c r="R439" s="3"/>
+      <c r="S439" s="3"/>
+      <c r="T439" s="3"/>
+      <c r="U439" s="3"/>
+      <c r="V439" s="3"/>
+    </row>
+    <row r="440" ht="45.0" customHeight="1">
+      <c r="A440" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="B440" s="3" t="s">
+        <v>704</v>
+      </c>
+      <c r="C440" s="3" t="s">
+        <v>701</v>
+      </c>
+      <c r="D440" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E440" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F440" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G440" s="18" t="s">
+        <v>707</v>
+      </c>
+      <c r="H440" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I440" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J440" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K440" s="3"/>
+      <c r="L440" s="3"/>
+      <c r="M440" s="3"/>
+      <c r="N440" s="3"/>
+      <c r="O440" s="3"/>
+      <c r="P440" s="3"/>
+      <c r="Q440" s="3"/>
+      <c r="R440" s="3"/>
+      <c r="S440" s="3"/>
+      <c r="T440" s="3"/>
+      <c r="U440" s="3"/>
+      <c r="V440" s="3"/>
+    </row>
+    <row r="441" ht="45.0" customHeight="1">
+      <c r="A441" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>709</v>
+      </c>
+      <c r="C441" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="D441" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E441" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F441" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G441" s="18" t="s">
+        <v>703</v>
+      </c>
+      <c r="H441" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I441" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J441" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K441" s="3"/>
+      <c r="L441" s="3"/>
+      <c r="M441" s="3"/>
+      <c r="N441" s="3"/>
+      <c r="O441" s="3"/>
+      <c r="P441" s="3"/>
+      <c r="Q441" s="3"/>
+      <c r="R441" s="3"/>
+      <c r="S441" s="3"/>
+      <c r="T441" s="3"/>
+      <c r="U441" s="3"/>
+      <c r="V441" s="3"/>
+    </row>
+    <row r="442" ht="45.0" customHeight="1">
+      <c r="A442" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="B442" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C442" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="D442" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E442" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F442" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G442" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="H442" s="3" t="s">
+        <v>705</v>
+      </c>
+      <c r="I442" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J442" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K442" s="3"/>
+      <c r="L442" s="3"/>
+      <c r="M442" s="3"/>
+      <c r="N442" s="3"/>
+      <c r="O442" s="3"/>
+      <c r="P442" s="3"/>
+      <c r="Q442" s="3"/>
+      <c r="R442" s="3"/>
+      <c r="S442" s="3"/>
+      <c r="T442" s="3"/>
+      <c r="U442" s="3"/>
+      <c r="V442" s="3"/>
+    </row>
+    <row r="443" ht="45.0" customHeight="1">
+      <c r="A443" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="B443" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="C443" s="3" t="s">
+        <v>708</v>
+      </c>
+      <c r="D443" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E443" s="3" t="s">
+        <v>706</v>
+      </c>
+      <c r="F443" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G443" s="18" t="s">
+        <v>707</v>
+      </c>
+      <c r="H443" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="I443" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="J443" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K443" s="3"/>
+      <c r="L443" s="3"/>
+      <c r="M443" s="3"/>
+      <c r="N443" s="3"/>
+      <c r="O443" s="3"/>
+      <c r="P443" s="3"/>
+      <c r="Q443" s="3"/>
+      <c r="R443" s="3"/>
+      <c r="S443" s="3"/>
+      <c r="T443" s="3"/>
+      <c r="U443" s="3"/>
+      <c r="V443" s="3"/>
+    </row>
     <row r="444" ht="45.0" customHeight="1"/>
     <row r="445" ht="45.0" customHeight="1"/>
     <row r="446" ht="45.0" customHeight="1"/>

</xml_diff>